<commit_message>
Update parts list for human sensing team
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="9520" yWindow="3940" windowWidth="18200" windowHeight="11060"/>
@@ -11,9 +11,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="130404" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -114,16 +114,50 @@
   </si>
   <si>
     <t>Date Ordered</t>
+  </si>
+  <si>
+    <t>Thermal Sensor</t>
+  </si>
+  <si>
+    <t>Omron D6T Thermal Sensor</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-highlights/us/en/omron-d6t-thermal-sensor/2745</t>
+  </si>
+  <si>
+    <t>Thermal sensor</t>
+  </si>
+  <si>
+    <t>8 includes 4 replacements</t>
+  </si>
+  <si>
+    <t>Temperature sensor</t>
+  </si>
+  <si>
+    <t>TMP36 - Analog Temperature sensor - TMP36</t>
+  </si>
+  <si>
+    <t>http://www.adafruit.com/products/165</t>
+  </si>
+  <si>
+    <t>Determine if thermal sensor readings should be disregarded</t>
+  </si>
+  <si>
+    <t>4 includes 3 replacements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +189,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,7 +222,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -186,6 +230,8 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -193,7 +239,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -488,18 +534,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.625" customWidth="1"/>
     <col min="2" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.375" customWidth="1"/>
     <col min="5" max="5" width="8.5" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
@@ -512,7 +559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="28">
+    <row r="3" spans="1:10" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -649,17 +696,57 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="E16" s="3"/>
-      <c r="F16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="5">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6">
+        <v>50</v>
+      </c>
+      <c r="F16" s="6">
+        <v>400</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="E17" s="3"/>
-      <c r="F17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="5">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6">
+        <v>2</v>
+      </c>
+      <c r="F17" s="6">
+        <v>8</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -875,7 +962,7 @@
       </c>
       <c r="F42" s="3">
         <f>SUM(F5:F41)</f>
-        <v>1204.99</v>
+        <v>1612.99</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -899,14 +986,14 @@
       </c>
       <c r="F46" s="3">
         <f>F42-F44</f>
-        <v>39.990000000000009</v>
+        <v>447.99</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -914,16 +1001,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -931,16 +1019,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Revert "Added Udoo processor"
This reverts commit 6e38a243544074d1dc40ceb4b4853214c498f976.
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9680" yWindow="5120" windowWidth="18200" windowHeight="11060"/>
+    <workbookView xWindow="9520" yWindow="3940" windowWidth="18200" windowHeight="11060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -114,27 +114,6 @@
   </si>
   <si>
     <t>Date Ordered</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>Udoo quad</t>
-  </si>
-  <si>
-    <t>http://shop.udoo.org/usa/product/udoo-quad.html</t>
-  </si>
-  <si>
-    <t>One for Human, one for SLAM</t>
-  </si>
-  <si>
-    <t>Accessories for Procesor</t>
-  </si>
-  <si>
-    <t>Udoo Accessory kit</t>
-  </si>
-  <si>
-    <t>http://shop.udoo.org/usa/catalog/product/view/id/34/s/starter-kit-usa/category/3/</t>
   </si>
 </sst>
 </file>
@@ -194,10 +173,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -210,11 +187,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -514,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -580,61 +555,29 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>135</v>
-      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F27" si="0">D5*E5</f>
-        <v>270</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="4">
-        <v>41673</v>
+        <f t="shared" ref="F5:F26" si="0">D5*E5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" s="3">
-        <v>29.99</v>
+        <v>0</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
-        <v>59.98</v>
-      </c>
-      <c r="G6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -655,6 +598,9 @@
       </c>
     </row>
     <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
@@ -662,9 +608,6 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3">
         <f t="shared" si="0"/>
@@ -693,6 +636,12 @@
       </c>
     </row>
     <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
@@ -700,12 +649,6 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
@@ -741,43 +684,43 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="E21" s="3"/>
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1165</v>
+      </c>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1165</v>
+      </c>
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="4">
+        <v>41670</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
       <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3">
-        <v>1165</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E22" s="3"/>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
-        <v>1165</v>
-      </c>
-      <c r="G22" t="s">
-        <v>27</v>
-      </c>
-      <c r="J22" s="4">
-        <v>41670</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3">
         <f t="shared" si="0"/>
@@ -799,58 +742,58 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="E26" s="3"/>
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
       <c r="F26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="G26" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" t="s">
-        <v>8</v>
-      </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" s="3">
-        <v>0</v>
+        <v>39.99</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D27*E27</f>
+        <v>39.99</v>
       </c>
       <c r="G27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3">
-        <v>39.99</v>
-      </c>
+      <c r="E28" s="3"/>
       <c r="F28" s="3">
-        <f>D28*E28</f>
-        <v>39.99</v>
-      </c>
-      <c r="G28" t="s">
-        <v>24</v>
+        <f t="shared" ref="F28:F40" si="1">D28*E28</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="E29" s="3"/>
       <c r="F29" s="3">
-        <f t="shared" ref="F29:F41" si="1">D29*E29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -875,98 +818,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:6">
       <c r="E33" s="3"/>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:6">
       <c r="E34" s="3"/>
       <c r="F34" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:6">
       <c r="E35" s="3"/>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
-      <c r="E36" s="3"/>
+    <row r="36" spans="1:6">
       <c r="F36" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:6">
       <c r="F37" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:6">
       <c r="F38" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:6">
       <c r="F39" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:6">
       <c r="F40" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
-      <c r="F41" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" t="s">
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
         <v>23</v>
       </c>
-      <c r="F43" s="3">
-        <f>SUM(F5:F42)</f>
-        <v>1534.97</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" t="s">
+      <c r="F42" s="3">
+        <f>SUM(F5:F41)</f>
+        <v>1204.99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
         <v>29</v>
       </c>
-      <c r="F45" s="3">
-        <f>SUM(F22)</f>
+      <c r="F44" s="3">
+        <f>SUM(F21)</f>
         <v>1165</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
-      <c r="F46" s="3"/>
-      <c r="J46" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" t="s">
+    <row r="45" spans="1:6">
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
         <v>28</v>
       </c>
-      <c r="F47" s="3">
-        <f>F43-F45</f>
-        <v>369.97</v>
+      <c r="F46" s="3">
+        <f>F42-F44</f>
+        <v>39.990000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited parts list, added mirrors and mirror mount structure
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Downloads\Vanderbilt\Junior Year_2013_2014\Spring Semester\UAV\GitRepository\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="3940" windowWidth="18200" windowHeight="11060"/>
+    <workbookView xWindow="9525" yWindow="3945" windowWidth="18195" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -162,6 +167,15 @@
   </si>
   <si>
     <t>http://shop.udoo.org/usa/catalog/product/view/id/34/s/starter-kit-usa/category/3/</t>
+  </si>
+  <si>
+    <t>Mirrors</t>
+  </si>
+  <si>
+    <t>Mirrors for LRF</t>
+  </si>
+  <si>
+    <t>Mirror Mount</t>
   </si>
 </sst>
 </file>
@@ -261,6 +275,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -555,28 +572,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="28">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -608,11 +625,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -639,7 +656,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>44</v>
       </c>
@@ -660,7 +677,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>20</v>
       </c>
@@ -675,66 +692,66 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <f>D11*E11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E12" s="3"/>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E13" s="3"/>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E14" s="3"/>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E15" s="3"/>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -747,7 +764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>31</v>
@@ -774,7 +791,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>36</v>
@@ -801,28 +818,28 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E19" s="3"/>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E20" s="3"/>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E21" s="3"/>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -849,38 +866,50 @@
         <v>41670</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <f>D23*E23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E26" s="3"/>
       <c r="F26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -901,7 +930,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>21</v>
       </c>
@@ -922,93 +951,93 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E29" s="3"/>
       <c r="F29" s="3">
         <f t="shared" ref="F29:F41" si="1">D29*E29</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E33" s="3"/>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E34" s="3"/>
       <c r="F34" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E35" s="3"/>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E36" s="3"/>
       <c r="F36" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F37" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F38" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F39" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F40" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F41" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -1017,10 +1046,10 @@
         <v>1942.97</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -1029,10 +1058,10 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -1059,7 +1088,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1076,7 +1105,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
removed IR sensors from SLAM
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Downloads\Vanderbilt\Junior Year_2013_2014\Spring Semester\UAV\GitRepository\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9525" yWindow="3945" windowWidth="18195" windowHeight="11055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -77,9 +72,6 @@
   </si>
   <si>
     <t>Laser Range Finder</t>
-  </si>
-  <si>
-    <t>Infrared sensors</t>
   </si>
   <si>
     <t>Kinect</t>
@@ -570,30 +562,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="28">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -622,14 +614,14 @@
         <v>14</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -637,7 +629,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -646,22 +638,22 @@
         <v>135</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F27" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F26" si="0">D5*E5</f>
         <v>270</v>
       </c>
       <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
         <v>42</v>
       </c>
-      <c r="H5" t="s">
+    </row>
+    <row r="6" spans="1:10">
+      <c r="B6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>45</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -674,12 +666,12 @@
         <v>59.98</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -692,28 +684,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -723,40 +715,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="E12" s="3"/>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="E13" s="3"/>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="E14" s="3"/>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="E15" s="3"/>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3">
@@ -764,13 +756,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D17" s="5">
         <v>8</v>
@@ -782,22 +774,22 @@
         <v>400</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="D18" s="5">
         <v>4</v>
@@ -809,37 +801,37 @@
         <v>8</v>
       </c>
       <c r="G18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10">
       <c r="E19" s="3"/>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="E20" s="3"/>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="E21" s="3"/>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -847,7 +839,7 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -860,220 +852,209 @@
         <v>1165</v>
       </c>
       <c r="G22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J22" s="4">
         <v>41670</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="B23" t="s">
-        <v>17</v>
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3">
-        <f>D23*E23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="C24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
+    <row r="25" spans="1:10">
       <c r="E25" s="3"/>
       <c r="F25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E26" s="3"/>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
       <c r="F26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>8</v>
-      </c>
+      <c r="G26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="B27" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" s="3">
-        <v>0</v>
+        <v>39.99</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D27*E27</f>
+        <v>39.99</v>
       </c>
       <c r="G27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3">
-        <v>39.99</v>
-      </c>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="E28" s="3"/>
       <c r="F28" s="3">
-        <f>D28*E28</f>
-        <v>39.99</v>
-      </c>
-      <c r="G28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F28:F40" si="1">D28*E28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="E29" s="3"/>
       <c r="F29" s="3">
-        <f t="shared" ref="F29:F41" si="1">D29*E29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="E30" s="3"/>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="E31" s="3"/>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="E32" s="3"/>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="E33" s="3"/>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="E34" s="3"/>
       <c r="F34" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="E35" s="3"/>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E36" s="3"/>
+    <row r="36" spans="1:6">
       <c r="F36" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="F37" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="F38" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="F39" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="F40" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F41" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>23</v>
-      </c>
-      <c r="F43" s="3">
-        <f>SUM(F5:F42)</f>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="3">
+        <f>SUM(F5:F41)</f>
         <v>1942.97</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>29</v>
-      </c>
-      <c r="F45" s="3">
+    <row r="43" spans="1:6">
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+      <c r="F44" s="3">
         <f>SUM(F22)</f>
         <v>1165</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>28</v>
-      </c>
-      <c r="F47" s="3">
-        <f>F43-F45</f>
+    <row r="45" spans="1:6">
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="3">
+        <f>F42-F44</f>
         <v>777.97</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1088,7 +1069,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1105,7 +1086,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Updated temp sensor purchase link.
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="14616"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -134,9 +134,6 @@
     <t>TMP36 - Analog Temperature sensor - TMP36</t>
   </si>
   <si>
-    <t>http://www.adafruit.com/products/165</t>
-  </si>
-  <si>
     <t>Determine if thermal sensor readings should be disregarded</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>Mirror Mount</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/TMP36GT9Z/TMP36GT9Z-ND/820404</t>
   </si>
 </sst>
 </file>
@@ -237,14 +237,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -254,12 +255,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -565,27 +568,27 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="3" width="27.5" customWidth="1"/>
+    <col min="2" max="3" width="27.44140625" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="28">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -617,11 +620,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -629,7 +632,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -642,18 +645,18 @@
         <v>270</v>
       </c>
       <c r="G5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" t="s">
         <v>41</v>
       </c>
-      <c r="H5" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>43</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -666,10 +669,10 @@
         <v>59.98</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -684,28 +687,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -715,35 +718,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E12" s="3"/>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E13" s="3"/>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E14" s="3"/>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E15" s="3"/>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -756,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>30</v>
@@ -783,7 +786,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>35</v>
@@ -795,43 +798,44 @@
         <v>4</v>
       </c>
       <c r="E18" s="6">
-        <v>2</v>
+        <v>1.42</v>
       </c>
       <c r="F18" s="6">
-        <v>8</v>
-      </c>
-      <c r="G18" s="5" t="s">
+        <f>D18*E18</f>
+        <v>5.68</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E19" s="3"/>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E20" s="3"/>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E21" s="3"/>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -858,12 +862,12 @@
         <v>41670</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -874,9 +878,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3">
@@ -884,14 +888,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E25" s="3"/>
       <c r="F25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -912,7 +916,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>20</v>
       </c>
@@ -933,105 +937,105 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E28" s="3"/>
       <c r="F28" s="3">
         <f t="shared" ref="F28:F40" si="1">D28*E28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E29" s="3"/>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E30" s="3"/>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E31" s="3"/>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E32" s="3"/>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E33" s="3"/>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E34" s="3"/>
       <c r="F34" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E35" s="3"/>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F36" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F37" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F38" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F39" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F40" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>22</v>
       </c>
       <c r="F42" s="3">
         <f>SUM(F5:F41)</f>
-        <v>1942.97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>1940.6499999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -1040,20 +1044,23 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>27</v>
       </c>
       <c r="F46" s="3">
         <f>F42-F44</f>
-        <v>777.97</v>
+        <v>775.64999999999986</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G18" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1069,7 +1076,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1086,7 +1093,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Demonstrating how to commit and push
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="14616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/TMP36GT9Z/TMP36GT9Z-ND/820404</t>
+  </si>
+  <si>
+    <t>Face plate</t>
   </si>
 </sst>
 </file>
@@ -568,27 +571,27 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="3" width="27.44140625" customWidth="1"/>
+    <col min="2" max="3" width="27.5" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="28">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -620,11 +623,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -651,7 +654,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" t="s">
         <v>42</v>
       </c>
@@ -672,7 +675,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -687,30 +690,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3">
@@ -718,35 +724,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="E12" s="3"/>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="E13" s="3"/>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="E14" s="3"/>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="E15" s="3"/>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -759,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>30</v>
@@ -786,7 +792,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>35</v>
@@ -814,28 +820,28 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="E19" s="3"/>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="E20" s="3"/>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="E21" s="3"/>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -862,7 +868,7 @@
         <v>41670</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="B23" t="s">
         <v>46</v>
       </c>
@@ -878,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="B24" t="s">
         <v>47</v>
       </c>
@@ -888,14 +894,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10">
       <c r="E25" s="3"/>
       <c r="F25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -916,7 +922,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="B27" t="s">
         <v>20</v>
       </c>
@@ -937,93 +943,93 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="E28" s="3"/>
       <c r="F28" s="3">
         <f t="shared" ref="F28:F40" si="1">D28*E28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10">
       <c r="E29" s="3"/>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10">
       <c r="E30" s="3"/>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="E31" s="3"/>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="E32" s="3"/>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="E33" s="3"/>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6">
       <c r="E34" s="3"/>
       <c r="F34" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="E35" s="3"/>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="F36" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6">
       <c r="F37" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="F38" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="F39" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="F40" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -1032,10 +1038,10 @@
         <v>1940.6499999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -1044,10 +1050,10 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>27</v>
       </c>
@@ -1076,7 +1082,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1093,7 +1099,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Revert "Demonstrating how to commit and push"
This reverts commit 86a8906a9d21d0d8cbacd58916a871abfca92524.
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="14616"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/TMP36GT9Z/TMP36GT9Z-ND/820404</t>
-  </si>
-  <si>
-    <t>Face plate</t>
   </si>
 </sst>
 </file>
@@ -571,27 +568,27 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="3" width="27.5" customWidth="1"/>
+    <col min="2" max="3" width="27.44140625" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="28">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -623,11 +620,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -654,7 +651,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>42</v>
       </c>
@@ -675,7 +672,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -690,33 +687,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3">
@@ -724,35 +718,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E12" s="3"/>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E13" s="3"/>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E14" s="3"/>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E15" s="3"/>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -765,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>30</v>
@@ -792,7 +786,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>35</v>
@@ -820,28 +814,28 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E19" s="3"/>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E20" s="3"/>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E21" s="3"/>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -868,7 +862,7 @@
         <v>41670</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>46</v>
       </c>
@@ -884,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>47</v>
       </c>
@@ -894,14 +888,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E25" s="3"/>
       <c r="F25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -922,7 +916,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>20</v>
       </c>
@@ -943,93 +937,93 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E28" s="3"/>
       <c r="F28" s="3">
         <f t="shared" ref="F28:F40" si="1">D28*E28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E29" s="3"/>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E30" s="3"/>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E31" s="3"/>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E32" s="3"/>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E33" s="3"/>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E34" s="3"/>
       <c r="F34" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E35" s="3"/>
       <c r="F35" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F36" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F37" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F38" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F39" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F40" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -1038,10 +1032,10 @@
         <v>1940.6499999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -1050,10 +1044,10 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>27</v>
       </c>
@@ -1082,7 +1076,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1099,7 +1093,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Wireless Network USB Adaptor choices
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="24240" windowHeight="13680"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="89">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -248,7 +248,46 @@
     <t>Solder and Wiring</t>
   </si>
   <si>
-    <t>Wifi receiver (Linux)</t>
+    <t>Wireless USB Adapter/Antenna</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/Wireless-Lan-Compat-W-Linux-Windows-Mac-Op-System-Standard-802-11B-G-w-Antenna-/331016562794?pt=US_USB_Wi_Fi_Adapters_Dongles&amp;hash=item4d121fe86a</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/Panda-Mid-Range-WiFi-150Mbps-802-11N-USB-Adapter-for-Windows-Mac-and-Linux-/121172036115</t>
+  </si>
+  <si>
+    <t>Wireless Lan,Linux,Windows,Mac Op System, Standard 802.11B/G w/Antenna</t>
+  </si>
+  <si>
+    <t>Panda Mid-Range WiFi 150Mbps 802.11N USB Adapter for Windows, Mac and Linux</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/Panda-Long-Range-WiFi-150Mbps-802-11N-USB-Adapter-for-Windows-Mac-and-Linux-/121172035907</t>
+  </si>
+  <si>
+    <t>Panda Long-Range WiFi 150Mbps 802.11N USB Adapter for Windows, Mac and Linux</t>
+  </si>
+  <si>
+    <t>For sensor data (vedio, image, map, etc.) transmission between UAV and off-board PC.  This wireless usb adapter is Linux compatible.  But the one we have in the lab is not Linux compatible.</t>
+  </si>
+  <si>
+    <t>One of the wireless USB adapter choice</t>
+  </si>
+  <si>
+    <t>300Mbps USB Wireless WiFi Adapter WiFi Network Lan Card With External Antenna US</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/300Mbps-USB-Wireless-WiFi-Adapter-WiFi-Network-Lan-Card-With-External-Antenna-US-/170985813126</t>
+  </si>
+  <si>
+    <t>Mini USB Wireless N 150Mbps Network Adapter For Windows VISTA WIN7 LINUX MAC</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/Mini-USB-Wireless-N-150Mbps-Network-Adapter-For-Windows-VISTA-WIN7-LINUX-MAC-/171152230954</t>
+  </si>
+  <si>
+    <t>One of the wireless USB adapter choice.  This one is mini adapter with light weight compare to other choices.</t>
   </si>
 </sst>
 </file>
@@ -258,7 +297,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +339,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -327,7 +373,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -338,6 +384,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -650,28 +697,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="28">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -703,11 +750,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -734,7 +781,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>42</v>
       </c>
@@ -755,7 +802,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -770,28 +817,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -801,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>49</v>
       </c>
@@ -822,7 +869,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>49</v>
       </c>
@@ -843,7 +890,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>54</v>
       </c>
@@ -864,7 +911,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>57</v>
       </c>
@@ -885,7 +932,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>59</v>
       </c>
@@ -906,7 +953,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>62</v>
       </c>
@@ -927,7 +974,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>64</v>
       </c>
@@ -948,7 +995,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>67</v>
       </c>
@@ -969,7 +1016,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>70</v>
       </c>
@@ -990,35 +1037,35 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E21" s="3"/>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E22" s="3"/>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>
       <c r="F23" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1031,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>30</v>
@@ -1058,7 +1105,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>35</v>
@@ -1086,28 +1133,28 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>
       <c r="F28" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E29" s="3"/>
       <c r="F29" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
       <c r="F30" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1134,7 +1181,7 @@
         <v>41670</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>46</v>
       </c>
@@ -1150,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>47</v>
       </c>
@@ -1160,14 +1207,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E34" s="3"/>
       <c r="F34" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1188,7 +1235,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>20</v>
       </c>
@@ -1209,7 +1256,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>72</v>
       </c>
@@ -1219,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>73</v>
       </c>
@@ -1229,9 +1276,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3">
@@ -1239,87 +1286,169 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>74</v>
-      </c>
-      <c r="E40" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3">
+        <v>24.47</v>
+      </c>
       <c r="F40" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="E41" s="3"/>
+        <v>24.47</v>
+      </c>
+      <c r="G40" t="s">
+        <v>76</v>
+      </c>
+      <c r="H40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3">
+        <v>14.99</v>
+      </c>
       <c r="F41" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="E42" s="3"/>
+        <v>14.99</v>
+      </c>
+      <c r="G41" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
+        <v>16.989999999999998</v>
+      </c>
       <c r="F42" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="E43" s="3"/>
+        <v>16.989999999999998</v>
+      </c>
+      <c r="G42" t="s">
+        <v>80</v>
+      </c>
+      <c r="H42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <v>8.56</v>
+      </c>
       <c r="F43" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="E44" s="3"/>
+        <v>8.56</v>
+      </c>
+      <c r="G43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3">
+        <v>6.39</v>
+      </c>
       <c r="F44" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>6.39</v>
+      </c>
+      <c r="G44" t="s">
+        <v>87</v>
+      </c>
+      <c r="H44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F45" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F46" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F47" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F48" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F49" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>22</v>
       </c>
       <c r="F51" s="3">
         <f>SUM(F5:F50)</f>
-        <v>2036.3700000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>2107.7699999999995</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>28</v>
       </c>
@@ -1328,16 +1457,16 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>27</v>
       </c>
       <c r="F55" s="3">
         <f>F51-F53</f>
-        <v>871.37000000000012</v>
+        <v>942.76999999999953</v>
       </c>
     </row>
   </sheetData>
@@ -1346,6 +1475,7 @@
     <hyperlink ref="G27" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1360,7 +1490,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1377,7 +1507,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Updated Parts list to include UDOO Camera
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Downloads\Vanderbilt\Junior Year_2013_2014\Spring Semester\UAV\GitRepository\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -288,6 +293,15 @@
   </si>
   <si>
     <t>One of the wireless USB adapter choice.  This one is mini adapter with light weight compare to other choices.</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>UDOO Autofocus Camera 5.0</t>
+  </si>
+  <si>
+    <t>http://shop.udoo.org/usa/accessories/autofocus-camera-5-0.html?___from_store=other&amp;popup=no</t>
   </si>
 </sst>
 </file>
@@ -451,7 +465,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -486,7 +500,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -695,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +785,7 @@
         <v>135</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F35" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F36" si="0">D5*E5</f>
         <v>270</v>
       </c>
       <c r="G5" t="s">
@@ -1208,77 +1222,88 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E34" s="3"/>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3">
+        <v>39</v>
+      </c>
       <c r="F34" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="G34" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="E35" s="3"/>
+      <c r="F35" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>8</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>18</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <v>2</v>
       </c>
-      <c r="E35" s="3">
-        <v>0</v>
-      </c>
-      <c r="F35" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" s="3">
-        <v>39.99</v>
-      </c>
-      <c r="F36" s="3">
-        <f>D36*E36</f>
-        <v>39.99</v>
-      </c>
-      <c r="G36" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3">
+        <v>39.99</v>
+      </c>
       <c r="F37" s="3">
-        <f t="shared" ref="F37:F49" si="2">D37*E37</f>
-        <v>0</v>
+        <f>D37*E37</f>
+        <v>39.99</v>
+      </c>
+      <c r="G37" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F38:F50" si="2">D38*E38</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3">
@@ -1288,26 +1313,12 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" s="3">
-        <v>24.47</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E40" s="3"/>
       <c r="F40" s="3">
         <f t="shared" si="2"/>
-        <v>24.47</v>
-      </c>
-      <c r="G40" t="s">
-        <v>76</v>
-      </c>
-      <c r="H40" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1315,23 +1326,23 @@
         <v>75</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" s="3">
-        <v>14.99</v>
+        <v>24.47</v>
       </c>
       <c r="F41" s="3">
         <f t="shared" si="2"/>
-        <v>14.99</v>
+        <v>24.47</v>
       </c>
       <c r="G41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1339,20 +1350,20 @@
         <v>75</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" s="3">
-        <v>16.989999999999998</v>
+        <v>14.99</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" si="2"/>
-        <v>16.989999999999998</v>
+        <v>14.99</v>
       </c>
       <c r="G42" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H42" t="s">
         <v>83</v>
@@ -1363,20 +1374,20 @@
         <v>75</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" s="3">
-        <v>8.56</v>
+        <v>16.989999999999998</v>
       </c>
       <c r="F43" s="3">
         <f t="shared" si="2"/>
-        <v>8.56</v>
+        <v>16.989999999999998</v>
       </c>
       <c r="G43" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H43" t="s">
         <v>83</v>
@@ -1387,29 +1398,47 @@
         <v>75</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" s="3">
-        <v>6.39</v>
+        <v>8.56</v>
       </c>
       <c r="F44" s="3">
         <f t="shared" si="2"/>
+        <v>8.56</v>
+      </c>
+      <c r="G44" t="s">
+        <v>85</v>
+      </c>
+      <c r="H44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3">
         <v>6.39</v>
       </c>
-      <c r="G44" t="s">
-        <v>87</v>
-      </c>
-      <c r="H44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F45" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.39</v>
+      </c>
+      <c r="G45" t="s">
+        <v>87</v>
+      </c>
+      <c r="H45" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1436,37 +1465,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>22</v>
       </c>
-      <c r="F51" s="3">
-        <f>SUM(F5:F50)</f>
-        <v>2107.7699999999995</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F52" s="3"/>
+      <c r="F52" s="3">
+        <f>SUM(F5:F51)</f>
+        <v>2146.7699999999991</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>28</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F54" s="3">
         <f>SUM(F31)</f>
         <v>1165</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F54" s="3"/>
-    </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>27</v>
       </c>
-      <c r="F55" s="3">
-        <f>F51-F53</f>
-        <v>942.76999999999953</v>
+      <c r="F56" s="3">
+        <f>F52-F54</f>
+        <v>981.76999999999907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
USB WiFi Options Update
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -251,45 +251,9 @@
     <t>Wireless USB Adapter/Antenna</t>
   </si>
   <si>
-    <t>http://www.ebay.com/itm/Wireless-Lan-Compat-W-Linux-Windows-Mac-Op-System-Standard-802-11B-G-w-Antenna-/331016562794?pt=US_USB_Wi_Fi_Adapters_Dongles&amp;hash=item4d121fe86a</t>
-  </si>
-  <si>
-    <t>http://www.ebay.com/itm/Panda-Mid-Range-WiFi-150Mbps-802-11N-USB-Adapter-for-Windows-Mac-and-Linux-/121172036115</t>
-  </si>
-  <si>
-    <t>Wireless Lan,Linux,Windows,Mac Op System, Standard 802.11B/G w/Antenna</t>
-  </si>
-  <si>
-    <t>Panda Mid-Range WiFi 150Mbps 802.11N USB Adapter for Windows, Mac and Linux</t>
-  </si>
-  <si>
-    <t>http://www.ebay.com/itm/Panda-Long-Range-WiFi-150Mbps-802-11N-USB-Adapter-for-Windows-Mac-and-Linux-/121172035907</t>
-  </si>
-  <si>
-    <t>Panda Long-Range WiFi 150Mbps 802.11N USB Adapter for Windows, Mac and Linux</t>
-  </si>
-  <si>
     <t>For sensor data (vedio, image, map, etc.) transmission between UAV and off-board PC.  This wireless usb adapter is Linux compatible.  But the one we have in the lab is not Linux compatible.</t>
   </si>
   <si>
-    <t>One of the wireless USB adapter choice</t>
-  </si>
-  <si>
-    <t>300Mbps USB Wireless WiFi Adapter WiFi Network Lan Card With External Antenna US</t>
-  </si>
-  <si>
-    <t>http://www.ebay.com/itm/300Mbps-USB-Wireless-WiFi-Adapter-WiFi-Network-Lan-Card-With-External-Antenna-US-/170985813126</t>
-  </si>
-  <si>
-    <t>Mini USB Wireless N 150Mbps Network Adapter For Windows VISTA WIN7 LINUX MAC</t>
-  </si>
-  <si>
-    <t>http://www.ebay.com/itm/Mini-USB-Wireless-N-150Mbps-Network-Adapter-For-Windows-VISTA-WIN7-LINUX-MAC-/171152230954</t>
-  </si>
-  <si>
-    <t>One of the wireless USB adapter choice.  This one is mini adapter with light weight compare to other choices.</t>
-  </si>
-  <si>
     <t>Camera</t>
   </si>
   <si>
@@ -324,6 +288,21 @@
   </si>
   <si>
     <t>RP-SMA Connector</t>
+  </si>
+  <si>
+    <t>High Power 802.11n Wireless Compact USB Adapter</t>
+  </si>
+  <si>
+    <t>http://www.planet.com.tw/en/product/product.php?id=37435#dl</t>
+  </si>
+  <si>
+    <t>http://www.netkrom.com/legado/airnet_300mb_802.11bgn_high_power_usb_adapter.php?id=indor&amp;item=productos</t>
+  </si>
+  <si>
+    <t>AIRNET 300 Mbps 802.11bgn High Power USB Adapter</t>
+  </si>
+  <si>
+    <t>One of the wireless USB adapter choice.  Compare to upper wireless USB adapter, it has 300Mbps speed for transfter RX data.</t>
   </si>
 </sst>
 </file>
@@ -333,7 +312,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +361,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF292929"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -412,7 +397,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -424,6 +409,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -739,28 +725,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="28">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -792,11 +778,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -816,14 +802,14 @@
         <f t="shared" ref="F5:F36" si="0">D5*E5</f>
         <v>270</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="7" t="s">
         <v>40</v>
       </c>
       <c r="H5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>42</v>
       </c>
@@ -844,7 +830,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -859,28 +845,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -890,7 +876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>49</v>
       </c>
@@ -911,7 +897,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>49</v>
       </c>
@@ -932,7 +918,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>54</v>
       </c>
@@ -953,7 +939,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>57</v>
       </c>
@@ -974,7 +960,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>59</v>
       </c>
@@ -995,7 +981,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>62</v>
       </c>
@@ -1016,7 +1002,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>64</v>
       </c>
@@ -1037,7 +1023,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>67</v>
       </c>
@@ -1058,7 +1044,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>70</v>
       </c>
@@ -1079,35 +1065,35 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E21" s="3"/>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E22" s="3"/>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>
       <c r="F23" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1120,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>30</v>
@@ -1147,7 +1133,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>35</v>
@@ -1175,28 +1161,28 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>
       <c r="F28" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E29" s="3"/>
       <c r="F29" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
       <c r="F30" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1223,7 +1209,7 @@
         <v>41670</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>46</v>
       </c>
@@ -1239,7 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>47</v>
       </c>
@@ -1249,12 +1235,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1267,17 +1253,17 @@
         <v>39</v>
       </c>
       <c r="G34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E35" s="3"/>
       <c r="F35" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1298,7 +1284,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>20</v>
       </c>
@@ -1319,7 +1305,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>72</v>
       </c>
@@ -1329,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>73</v>
       </c>
@@ -1339,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>74</v>
       </c>
@@ -1349,211 +1335,147 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>78</v>
+      <c r="C41" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" s="3">
-        <v>24.47</v>
+        <v>23.75</v>
       </c>
       <c r="F41" s="3">
         <f t="shared" si="2"/>
-        <v>24.47</v>
-      </c>
-      <c r="G41" t="s">
+        <v>23.75</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H41" t="s">
         <v>76</v>
       </c>
-      <c r="H41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>75</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" s="3">
-        <v>14.99</v>
+        <v>13.78</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" si="2"/>
-        <v>14.99</v>
-      </c>
-      <c r="G42" t="s">
-        <v>77</v>
+        <v>13.78</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="H42" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
         <v>81</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" s="3">
-        <v>16.989999999999998</v>
+        <v>34.950000000000003</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" si="2"/>
-        <v>16.989999999999998</v>
+        <f>D43*E43</f>
+        <v>34.950000000000003</v>
       </c>
       <c r="G43" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H43" t="s">
+        <v>87</v>
+      </c>
+      <c r="I43" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="8" t="s">
         <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>86</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" s="3">
-        <v>8.56</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="F44" s="3">
-        <f t="shared" si="2"/>
-        <v>8.56</v>
+        <f>D44*E44</f>
+        <v>9.9499999999999993</v>
       </c>
       <c r="G44" t="s">
         <v>85</v>
       </c>
       <c r="H44" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="B45" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" s="3">
-        <v>6.39</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="I44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" s="8"/>
+      <c r="E45" s="3"/>
       <c r="F45" s="3">
         <f t="shared" si="2"/>
-        <v>6.39</v>
-      </c>
-      <c r="G45" t="s">
-        <v>87</v>
-      </c>
-      <c r="H45" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="B46" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" s="3">
-        <v>34.950000000000003</v>
-      </c>
-      <c r="F46" s="3">
-        <f t="shared" si="2"/>
-        <v>34.950000000000003</v>
-      </c>
-      <c r="G46" t="s">
-        <v>94</v>
-      </c>
-      <c r="H46" t="s">
-        <v>99</v>
-      </c>
-      <c r="I46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="B47" t="s">
-        <v>96</v>
-      </c>
-      <c r="C47" t="s">
-        <v>98</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47" s="3">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="F47" s="3">
-        <f t="shared" si="2"/>
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="G47" t="s">
-        <v>97</v>
-      </c>
-      <c r="H47" t="s">
-        <v>99</v>
-      </c>
-      <c r="I47" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F48" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F49" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F50" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>22</v>
       </c>
       <c r="F52" s="3">
         <f>SUM(F5:F51)</f>
-        <v>2191.6699999999987</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>2157.7999999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>28</v>
       </c>
@@ -1562,25 +1484,28 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>27</v>
       </c>
       <c r="F56" s="3">
         <f>F52-F54</f>
-        <v>1026.6699999999987</v>
+        <v>992.79999999999973</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G27" r:id="rId1"/>
+    <hyperlink ref="G41" r:id="rId2" location="dl"/>
+    <hyperlink ref="G42" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1595,7 +1520,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1612,7 +1537,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
updated thermal sensor information
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24600" windowHeight="15720"/>
+    <workbookView xWindow="780" yWindow="1100" windowWidth="24600" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Omron D6T Thermal Sensor</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-highlights/us/en/omron-d6t-thermal-sensor/2745</t>
-  </si>
-  <si>
     <t>Thermal sensor</t>
   </si>
   <si>
@@ -303,6 +300,12 @@
   </si>
   <si>
     <t>One of the wireless USB adapter choice.  Compare to upper wireless USB adapter, it has 300Mbps speed for transfter RX data.</t>
+  </si>
+  <si>
+    <t>received</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/D6T8L06/Z3638-ND/3671588</t>
   </si>
 </sst>
 </file>
@@ -737,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -802,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -815,18 +818,18 @@
         <v>270</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
         <v>40</v>
-      </c>
-      <c r="H5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
         <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -839,7 +842,7 @@
         <v>59.98</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -890,10 +893,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
         <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>50</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -906,15 +909,15 @@
         <v>7.81</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="B13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -927,15 +930,15 @@
         <v>7.81</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
         <v>54</v>
-      </c>
-      <c r="C14" t="s">
-        <v>55</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -948,15 +951,15 @@
         <v>15.62</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -969,15 +972,15 @@
         <v>40.4</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
         <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -990,15 +993,15 @@
         <v>6.72</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17">
         <v>4</v>
@@ -1011,15 +1014,15 @@
         <v>11.6</v>
       </c>
       <c r="G17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
         <v>64</v>
-      </c>
-      <c r="C18" t="s">
-        <v>65</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -1032,15 +1035,15 @@
         <v>5.76</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
         <v>67</v>
-      </c>
-      <c r="C19" t="s">
-        <v>68</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -1053,15 +1056,15 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
         <v>70</v>
-      </c>
-      <c r="C20" t="s">
-        <v>71</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -1074,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1121,6 +1124,9 @@
       <c r="F25" s="3">
         <f t="shared" si="0"/>
         <v>144.13999999999999</v>
+      </c>
+      <c r="J25" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1132,7 +1138,7 @@
         <v>31</v>
       </c>
       <c r="D26" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E26" s="6">
         <v>50</v>
@@ -1141,22 +1147,25 @@
         <v>400</v>
       </c>
       <c r="G26" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>34</v>
+      <c r="J26" s="4">
+        <v>41681</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="D27" s="5">
         <v>4</v>
@@ -1169,13 +1178,16 @@
         <v>5.68</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>38</v>
+      <c r="J27" s="4">
+        <v>41681</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1228,10 +1240,10 @@
     </row>
     <row r="32" spans="1:10">
       <c r="B32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -1244,7 +1256,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="B33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3">
@@ -1254,10 +1266,10 @@
     </row>
     <row r="34" spans="1:9">
       <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" t="s">
         <v>77</v>
-      </c>
-      <c r="C34" t="s">
-        <v>78</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1270,7 +1282,7 @@
         <v>39</v>
       </c>
       <c r="G34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1324,7 +1336,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="B38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3">
@@ -1334,7 +1346,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="B39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3">
@@ -1344,7 +1356,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="B40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3">
@@ -1354,10 +1366,10 @@
     </row>
     <row r="41" spans="1:9" s="10" customFormat="1">
       <c r="B41" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>81</v>
       </c>
       <c r="D41" s="10">
         <v>1</v>
@@ -1370,21 +1382,21 @@
         <v>34.950000000000003</v>
       </c>
       <c r="G41" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I41" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="B42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1397,13 +1409,13 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="G42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H42" t="s">
+        <v>86</v>
+      </c>
+      <c r="I42" t="s">
         <v>87</v>
-      </c>
-      <c r="I42" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1467,10 +1479,10 @@
     </row>
     <row r="65" spans="2:8">
       <c r="B65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -1483,18 +1495,18 @@
         <v>23.75</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H65" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="2:8">
       <c r="B66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -1507,10 +1519,10 @@
         <v>13.78</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated parts to have voltage regulator
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1100" windowWidth="24600" windowHeight="15720"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="106">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -324,6 +324,21 @@
   </si>
   <si>
     <t>http://www.hobbyking.com/hobbyking/store/__11176__Turnigy_450_H2218_Brushless_outrunner_1860KV.html</t>
+  </si>
+  <si>
+    <t>Voltage Regulators</t>
+  </si>
+  <si>
+    <t>TI LM2937ET-5.0/NOPB-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/LM2937ET-5.0%2FNOPB/LM2937ET-5.0%2FNOPB-ND/212651</t>
+  </si>
+  <si>
+    <t>In case of Udoo brownout</t>
+  </si>
+  <si>
+    <t>Through hole, tv, 500 mA max output supply</t>
   </si>
 </sst>
 </file>
@@ -786,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1501,11 +1516,30 @@
       </c>
     </row>
     <row r="43" spans="1:10">
-      <c r="C43" s="8"/>
-      <c r="E43" s="3"/>
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1.61</v>
+      </c>
       <c r="F43" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="G43" t="s">
+        <v>103</v>
+      </c>
+      <c r="H43" t="s">
+        <v>104</v>
+      </c>
+      <c r="I43" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1532,7 +1566,7 @@
       </c>
       <c r="F50" s="3">
         <f>SUM(F5:F49)</f>
-        <v>2417.2599999999993</v>
+        <v>2425.3099999999995</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1556,7 +1590,7 @@
       </c>
       <c r="F54" s="3">
         <f>F50-F52</f>
-        <v>1252.2599999999993</v>
+        <v>1260.3099999999995</v>
       </c>
     </row>
     <row r="65" spans="2:8">

</xml_diff>

<commit_message>
updated blades for Hobby Express
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1100" windowWidth="24600" windowHeight="15720"/>
+    <workbookView xWindow="820" yWindow="0" windowWidth="24600" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -311,9 +311,6 @@
     <t>In House</t>
   </si>
   <si>
-    <t>http://www.hobbyking.com/hobbyking/store/__43850__11x4_5E_Nylon_Multi_Rotor_Propellers_L_H_and_R_H_Rotation_2_pairs_.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">US </t>
   </si>
   <si>
@@ -339,6 +336,15 @@
   </si>
   <si>
     <t>Through hole, tv, 500 mA max output supply</t>
+  </si>
+  <si>
+    <t>http://www.hobbyexpress.com/gemfan_11x4.7_reverse_carbon_filled_1041840_prd1.htm?pSearchQueryId=4684805</t>
+  </si>
+  <si>
+    <t>Blades opposite direction</t>
+  </si>
+  <si>
+    <t>http://www.hobbyexpress.com/gemfan_11x4.7_normal_carbon_filled_1041839_prd1.htm?pSearchQueryId=4684805</t>
   </si>
 </sst>
 </file>
@@ -427,13 +433,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -471,7 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -494,6 +508,14 @@
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -801,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -960,7 +982,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
         <v>48</v>
@@ -984,7 +1006,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
         <v>48</v>
@@ -1008,7 +1030,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
         <v>53</v>
@@ -1032,7 +1054,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
         <v>56</v>
@@ -1056,7 +1078,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" t="s">
         <v>58</v>
@@ -1080,7 +1102,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" t="s">
         <v>61</v>
@@ -1104,7 +1126,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" t="s">
         <v>63</v>
@@ -1128,7 +1150,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
         <v>66</v>
@@ -1147,13 +1169,10 @@
         <v>133.4</v>
       </c>
       <c r="G19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" t="s">
-        <v>98</v>
-      </c>
       <c r="B20" t="s">
         <v>68</v>
       </c>
@@ -1164,21 +1183,32 @@
         <v>5</v>
       </c>
       <c r="E20" s="3">
-        <v>3.89</v>
+        <v>3</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="1"/>
-        <v>19.45</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="E21" s="3"/>
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21" s="3">
+        <v>3</v>
+      </c>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G21" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1517,10 +1547,10 @@
     </row>
     <row r="43" spans="1:10">
       <c r="B43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>102</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -1533,13 +1563,13 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="G43" t="s">
+        <v>102</v>
+      </c>
+      <c r="H43" t="s">
         <v>103</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>104</v>
-      </c>
-      <c r="I43" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1566,7 +1596,7 @@
       </c>
       <c r="F50" s="3">
         <f>SUM(F5:F49)</f>
-        <v>2425.3099999999995</v>
+        <v>2435.8599999999997</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1590,7 +1620,7 @@
       </c>
       <c r="F54" s="3">
         <f>F50-F52</f>
-        <v>1260.3099999999995</v>
+        <v>1270.8599999999997</v>
       </c>
     </row>
     <row r="65" spans="2:8">

</xml_diff>

<commit_message>
updated motors added speed controllers.
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Rotor Blades</t>
   </si>
   <si>
-    <t>ESC</t>
-  </si>
-  <si>
     <t>Power Distribution Board</t>
   </si>
   <si>
@@ -311,18 +308,6 @@
     <t>In House</t>
   </si>
   <si>
-    <t xml:space="preserve">US </t>
-  </si>
-  <si>
-    <t>International</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>http://www.hobbyking.com/hobbyking/store/__11176__Turnigy_450_H2218_Brushless_outrunner_1860KV.html</t>
-  </si>
-  <si>
     <t>Voltage Regulators</t>
   </si>
   <si>
@@ -345,6 +330,21 @@
   </si>
   <si>
     <t>http://www.hobbyexpress.com/gemfan_11x4.7_normal_carbon_filled_1041839_prd1.htm?pSearchQueryId=4684805</t>
+  </si>
+  <si>
+    <t>http://hobbyking.com/hobbyking/store/__26486__NTM_Prop_Drive_Series_35_36A_1800Kv_875w_US_Warehouse_.html</t>
+  </si>
+  <si>
+    <t>http://www.hobbyexpress.com/erc_rapid_drive_35a_brushless_esc_1039744_prd1.htm</t>
+  </si>
+  <si>
+    <t>35A</t>
+  </si>
+  <si>
+    <t>Returned</t>
+  </si>
+  <si>
+    <t>ESC - Speed Controllers</t>
   </si>
 </sst>
 </file>
@@ -433,13 +433,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="34">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -485,7 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="34">
+  <cellStyles count="36">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -516,6 +518,8 @@
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -823,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -907,7 +911,7 @@
         <v>40</v>
       </c>
       <c r="J5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -931,7 +935,7 @@
         <v>43</v>
       </c>
       <c r="J6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -981,9 +985,6 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>96</v>
-      </c>
       <c r="B12" t="s">
         <v>48</v>
       </c>
@@ -1003,11 +1004,11 @@
       <c r="G12" t="s">
         <v>50</v>
       </c>
+      <c r="J12" s="4">
+        <v>41684</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>98</v>
-      </c>
       <c r="B13" t="s">
         <v>48</v>
       </c>
@@ -1027,11 +1028,11 @@
       <c r="G13" t="s">
         <v>52</v>
       </c>
+      <c r="J13" s="4">
+        <v>41684</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>98</v>
-      </c>
       <c r="B14" t="s">
         <v>53</v>
       </c>
@@ -1051,11 +1052,11 @@
       <c r="G14" t="s">
         <v>55</v>
       </c>
+      <c r="J14" s="4">
+        <v>41684</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>98</v>
-      </c>
       <c r="B15" t="s">
         <v>56</v>
       </c>
@@ -1075,11 +1076,11 @@
       <c r="G15" t="s">
         <v>57</v>
       </c>
+      <c r="J15" s="4">
+        <v>41684</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>98</v>
-      </c>
       <c r="B16" t="s">
         <v>58</v>
       </c>
@@ -1099,11 +1100,11 @@
       <c r="G16" t="s">
         <v>60</v>
       </c>
+      <c r="J16" s="4">
+        <v>41684</v>
+      </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>98</v>
-      </c>
       <c r="B17" t="s">
         <v>61</v>
       </c>
@@ -1123,11 +1124,11 @@
       <c r="G17" t="s">
         <v>62</v>
       </c>
+      <c r="J17" s="4">
+        <v>41684</v>
+      </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" t="s">
-        <v>98</v>
-      </c>
       <c r="B18" t="s">
         <v>63</v>
       </c>
@@ -1147,11 +1148,11 @@
       <c r="G18" t="s">
         <v>65</v>
       </c>
+      <c r="J18" s="4">
+        <v>41684</v>
+      </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" t="s">
-        <v>97</v>
-      </c>
       <c r="B19" t="s">
         <v>66</v>
       </c>
@@ -1159,17 +1160,20 @@
         <v>67</v>
       </c>
       <c r="D19">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E19" s="3">
-        <v>13.34</v>
+        <v>18.48</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="1"/>
-        <v>133.4</v>
+        <v>110.88</v>
       </c>
       <c r="G19" t="s">
-        <v>99</v>
+        <v>103</v>
+      </c>
+      <c r="J19" s="4">
+        <v>41684</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1190,12 +1194,12 @@
         <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="B21" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -1208,7 +1212,7 @@
         <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1250,7 +1254,7 @@
         <v>144.13999999999999</v>
       </c>
       <c r="J25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1271,7 +1275,7 @@
         <v>400</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>32</v>
@@ -1359,7 +1363,7 @@
         <v>26</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1390,10 +1394,10 @@
     </row>
     <row r="34" spans="1:10">
       <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" t="s">
         <v>75</v>
-      </c>
-      <c r="C34" t="s">
-        <v>76</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1406,7 +1410,7 @@
         <v>39</v>
       </c>
       <c r="G34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1437,7 +1441,7 @@
         <v>24</v>
       </c>
       <c r="J36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1448,32 +1452,46 @@
         <v>21</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" s="3">
         <v>39.99</v>
       </c>
       <c r="F37" s="3">
         <f>D37*E37</f>
-        <v>39.99</v>
+        <v>0</v>
       </c>
       <c r="G37" t="s">
         <v>23</v>
       </c>
+      <c r="J37" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="38" spans="1:10">
       <c r="B38" t="s">
-        <v>70</v>
-      </c>
-      <c r="E38" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="C38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38" s="3">
+        <v>29.99</v>
+      </c>
       <c r="F38" s="3">
         <f t="shared" ref="F38:F48" si="2">D38*E38</f>
-        <v>0</v>
+        <v>149.94999999999999</v>
+      </c>
+      <c r="G38" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="B39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3">
@@ -1483,7 +1501,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="B40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3">
@@ -1493,10 +1511,10 @@
     </row>
     <row r="41" spans="1:10" s="10" customFormat="1">
       <c r="B41" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>79</v>
       </c>
       <c r="D41" s="10">
         <v>1</v>
@@ -1509,21 +1527,21 @@
         <v>34.950000000000003</v>
       </c>
       <c r="G41" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I41" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="B42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1536,21 +1554,21 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="G42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H42" t="s">
+        <v>84</v>
+      </c>
+      <c r="I42" t="s">
         <v>85</v>
-      </c>
-      <c r="I42" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="B43" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -1563,13 +1581,13 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="G43" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H43" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I43" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1596,7 +1614,7 @@
       </c>
       <c r="F50" s="3">
         <f>SUM(F5:F49)</f>
-        <v>2435.8599999999997</v>
+        <v>2523.2999999999997</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1620,15 +1638,15 @@
       </c>
       <c r="F54" s="3">
         <f>F50-F52</f>
-        <v>1270.8599999999997</v>
+        <v>1358.2999999999997</v>
       </c>
     </row>
     <row r="65" spans="2:8">
       <c r="B65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -1641,18 +1659,18 @@
         <v>23.75</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="2:8">
       <c r="B66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -1665,10 +1683,10 @@
         <v>13.78</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated quantities and order dates
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -433,7 +433,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -470,8 +470,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -486,8 +487,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="36">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -520,6 +522,7 @@
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -827,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -992,14 +995,14 @@
         <v>49</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3">
         <v>7.81</v>
       </c>
       <c r="F12" s="3">
         <f>D12*E12</f>
-        <v>7.81</v>
+        <v>15.62</v>
       </c>
       <c r="G12" t="s">
         <v>50</v>
@@ -1016,14 +1019,14 @@
         <v>51</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="3">
         <v>7.81</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" ref="F13:F20" si="1">D13*E13</f>
-        <v>7.81</v>
+        <v>15.62</v>
       </c>
       <c r="G13" t="s">
         <v>52</v>
@@ -1040,14 +1043,14 @@
         <v>54</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3">
         <v>7.81</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>15.62</v>
+        <v>31.24</v>
       </c>
       <c r="G14" t="s">
         <v>55</v>
@@ -1064,14 +1067,14 @@
         <v>56</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E15" s="3">
         <v>10.1</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>40.4</v>
+        <v>80.8</v>
       </c>
       <c r="G15" t="s">
         <v>57</v>
@@ -1088,14 +1091,14 @@
         <v>59</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E16" s="3">
         <v>1.68</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>6.72</v>
+        <v>13.44</v>
       </c>
       <c r="G16" t="s">
         <v>60</v>
@@ -1112,14 +1115,14 @@
         <v>61</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E17" s="3">
         <v>2.9</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="1"/>
-        <v>11.6</v>
+        <v>23.2</v>
       </c>
       <c r="G17" t="s">
         <v>62</v>
@@ -1136,14 +1139,14 @@
         <v>64</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E18" s="3">
         <v>1.44</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
-        <v>5.76</v>
+        <v>11.52</v>
       </c>
       <c r="G18" t="s">
         <v>65</v>
@@ -1160,14 +1163,14 @@
         <v>67</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E19" s="3">
         <v>18.48</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="1"/>
-        <v>110.88</v>
+        <v>184.8</v>
       </c>
       <c r="G19" t="s">
         <v>103</v>
@@ -1476,14 +1479,14 @@
         <v>105</v>
       </c>
       <c r="D38">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E38" s="3">
         <v>29.99</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" ref="F38:F48" si="2">D38*E38</f>
-        <v>149.94999999999999</v>
+        <v>179.94</v>
       </c>
       <c r="G38" t="s">
         <v>104</v>
@@ -1517,14 +1520,14 @@
         <v>78</v>
       </c>
       <c r="D41" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41" s="11">
         <v>34.950000000000003</v>
       </c>
       <c r="F41" s="11">
         <f>D41*E41</f>
-        <v>34.950000000000003</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="G41" s="10" t="s">
         <v>79</v>
@@ -1534,6 +1537,9 @@
       </c>
       <c r="I41" s="10" t="s">
         <v>80</v>
+      </c>
+      <c r="J41" s="12">
+        <v>41684</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1544,14 +1550,14 @@
         <v>83</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" s="3">
         <v>9.9499999999999993</v>
       </c>
       <c r="F42" s="3">
         <f>D42*E42</f>
-        <v>9.9499999999999993</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="G42" t="s">
         <v>82</v>
@@ -1561,6 +1567,9 @@
       </c>
       <c r="I42" t="s">
         <v>85</v>
+      </c>
+      <c r="J42" s="12">
+        <v>41684</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1571,14 +1580,14 @@
         <v>96</v>
       </c>
       <c r="D43">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E43" s="3">
-        <v>1.61</v>
+        <v>1.46</v>
       </c>
       <c r="F43" s="3">
         <f t="shared" si="2"/>
-        <v>8.0500000000000007</v>
+        <v>14.6</v>
       </c>
       <c r="G43" t="s">
         <v>97</v>
@@ -1588,6 +1597,9 @@
       </c>
       <c r="I43" t="s">
         <v>99</v>
+      </c>
+      <c r="J43" s="12">
+        <v>41684</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1614,7 +1626,7 @@
       </c>
       <c r="F50" s="3">
         <f>SUM(F5:F49)</f>
-        <v>2523.2999999999997</v>
+        <v>2774.38</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1638,7 +1650,7 @@
       </c>
       <c r="F54" s="3">
         <f>F50-F52</f>
-        <v>1358.2999999999997</v>
+        <v>1609.38</v>
       </c>
     </row>
     <row r="65" spans="2:8">

</xml_diff>

<commit_message>
Added Power Distro Board, Barrel Plugs, BEC
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="0" windowWidth="24600" windowHeight="15720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="117">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -345,6 +345,33 @@
   </si>
   <si>
     <t>ESC - Speed Controllers</t>
+  </si>
+  <si>
+    <t>https://store.3drobotics.com/products/quadcopter-power-distribution-board-1</t>
+  </si>
+  <si>
+    <t>Battery Eliminating Circuit</t>
+  </si>
+  <si>
+    <t>Barrel Plugs</t>
+  </si>
+  <si>
+    <t>9v battery clip to 5.5/2.2mm plug</t>
+  </si>
+  <si>
+    <t>http://www.adafruit.com/products/80</t>
+  </si>
+  <si>
+    <t>http://www.pololu.com/product/2177</t>
+  </si>
+  <si>
+    <t>5V 3A BEC Step-Down Voltage Regulator</t>
+  </si>
+  <si>
+    <t>3DR Quad Power Distribution Board</t>
+  </si>
+  <si>
+    <t>TBA</t>
   </si>
 </sst>
 </file>
@@ -828,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1472,101 +1499,89 @@
       </c>
     </row>
     <row r="38" spans="1:10">
-      <c r="B38" t="s">
-        <v>107</v>
-      </c>
       <c r="C38" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38">
-        <v>6</v>
-      </c>
-      <c r="E38" s="3">
-        <v>29.99</v>
-      </c>
-      <c r="F38" s="3">
-        <f t="shared" ref="F38:F48" si="2">D38*E38</f>
-        <v>179.94</v>
-      </c>
-      <c r="G38" t="s">
-        <v>104</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:10">
       <c r="B39" t="s">
-        <v>70</v>
-      </c>
-      <c r="E39" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="C39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+      <c r="E39" s="3">
+        <v>29.99</v>
+      </c>
       <c r="F39" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="F39:F49" si="2">D39*E39</f>
+        <v>179.94</v>
+      </c>
+      <c r="G39" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="B40" t="s">
-        <v>71</v>
-      </c>
-      <c r="E40" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="C40" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3">
+        <v>15</v>
+      </c>
       <c r="F40" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="10" customFormat="1">
-      <c r="B41" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="10" customFormat="1">
+      <c r="B42" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C42" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D42" s="10">
         <v>2</v>
       </c>
-      <c r="E41" s="11">
+      <c r="E42" s="11">
         <v>34.950000000000003</v>
       </c>
-      <c r="F41" s="11">
-        <f>D41*E41</f>
+      <c r="F42" s="11">
+        <f>D42*E42</f>
         <v>69.900000000000006</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G42" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="H42" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="I41" s="10" t="s">
+      <c r="I42" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="J41" s="12">
-        <v>41684</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="B42" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" t="s">
-        <v>83</v>
-      </c>
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42" s="3">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="F42" s="3">
-        <f>D42*E42</f>
-        <v>19.899999999999999</v>
-      </c>
-      <c r="G42" t="s">
-        <v>82</v>
-      </c>
-      <c r="H42" t="s">
-        <v>84</v>
-      </c>
-      <c r="I42" t="s">
-        <v>85</v>
       </c>
       <c r="J42" s="12">
         <v>41684</v>
@@ -1574,38 +1589,104 @@
     </row>
     <row r="43" spans="1:10">
       <c r="B43" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43" s="3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F43" s="3">
+        <f>D43*E43</f>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G43" t="s">
+        <v>82</v>
+      </c>
+      <c r="H43" t="s">
+        <v>84</v>
+      </c>
+      <c r="I43" t="s">
+        <v>85</v>
+      </c>
+      <c r="J43" s="12">
+        <v>41684</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="B44" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C44" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <v>10</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E44" s="3">
         <v>1.46</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F44" s="3">
         <f t="shared" si="2"/>
         <v>14.6</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G44" t="s">
         <v>97</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H44" t="s">
         <v>98</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I44" t="s">
         <v>99</v>
       </c>
-      <c r="J43" s="12">
+      <c r="J44" s="12">
         <v>41684</v>
       </c>
     </row>
+    <row r="45" spans="1:10">
+      <c r="B45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3">
+        <v>11.95</v>
+      </c>
+      <c r="F45" s="3">
+        <f t="shared" si="2"/>
+        <v>11.95</v>
+      </c>
+      <c r="G45" t="s">
+        <v>113</v>
+      </c>
+    </row>
     <row r="46" spans="1:10">
+      <c r="B46" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" s="3">
+        <v>3</v>
+      </c>
       <c r="F46" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>E46*D46</f>
+        <v>6</v>
+      </c>
+      <c r="G46" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -1620,84 +1701,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" t="s">
+    <row r="49" spans="1:6">
+      <c r="F49" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
         <v>22</v>
       </c>
-      <c r="F50" s="3">
-        <f>SUM(F5:F49)</f>
-        <v>2774.38</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="F51" s="3"/>
+      <c r="F51" s="3">
+        <f>SUM(F5:F50)</f>
+        <v>2807.33</v>
+      </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" t="s">
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
         <v>28</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F53" s="3">
         <f>SUM(F31)</f>
         <v>1165</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="F53" s="3"/>
-    </row>
     <row r="54" spans="1:6">
-      <c r="A54" t="s">
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
         <v>27</v>
       </c>
-      <c r="F54" s="3">
-        <f>F50-F52</f>
-        <v>1609.38</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8">
-      <c r="B65" t="s">
-        <v>72</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-      <c r="E65" s="3">
-        <v>23.75</v>
-      </c>
-      <c r="F65" s="3">
-        <f>D65*E65</f>
-        <v>23.75</v>
-      </c>
-      <c r="G65" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H65" t="s">
-        <v>73</v>
+      <c r="F55" s="3">
+        <f>F51-F53</f>
+        <v>1642.33</v>
       </c>
     </row>
     <row r="66" spans="2:8">
       <c r="B66" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="8" t="s">
-        <v>89</v>
+      <c r="C66" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66" s="3">
-        <v>13.78</v>
+        <v>23.75</v>
       </c>
       <c r="F66" s="3">
         <f>D66*E66</f>
+        <v>23.75</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H66" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8">
+      <c r="B67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" s="3">
         <v>13.78</v>
       </c>
-      <c r="G66" s="7" t="s">
+      <c r="F67" s="3">
+        <f>D67*E67</f>
+        <v>13.78</v>
+      </c>
+      <c r="G67" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H67" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1705,9 +1792,10 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G27" r:id="rId1"/>
-    <hyperlink ref="G65" r:id="rId2" location="dl"/>
-    <hyperlink ref="G66" r:id="rId3"/>
+    <hyperlink ref="G66" r:id="rId2" location="dl"/>
+    <hyperlink ref="G67" r:id="rId3"/>
     <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="C45" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updating Human Sensing parts
add IR sensor connectors/housings
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="128">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -375,6 +375,36 @@
   </si>
   <si>
     <t>Protoboards</t>
+  </si>
+  <si>
+    <t>Thermal Sensor Connectors</t>
+  </si>
+  <si>
+    <t>SSHL-002T-P0.2</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/SSHL-002T-P0.2/455-1606-1-ND/1642795</t>
+  </si>
+  <si>
+    <t>Connector for IR</t>
+  </si>
+  <si>
+    <t>10 includes replacements</t>
+  </si>
+  <si>
+    <t>Thermal Sensor Housing</t>
+  </si>
+  <si>
+    <t>GHR-04V-S</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/GHR-04V-S/455-1594-ND/807816</t>
+  </si>
+  <si>
+    <t>Housing for IR</t>
+  </si>
+  <si>
+    <t>8 Includes replacements</t>
   </si>
 </sst>
 </file>
@@ -862,28 +892,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="3" width="27.5" customWidth="1"/>
+    <col min="2" max="3" width="27.44140625" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="28">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -915,11 +945,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -949,7 +979,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>41</v>
       </c>
@@ -973,7 +1003,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -988,28 +1018,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1019,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>48</v>
       </c>
@@ -1043,7 +1073,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>48</v>
       </c>
@@ -1067,7 +1097,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>53</v>
       </c>
@@ -1091,7 +1121,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>56</v>
       </c>
@@ -1115,7 +1145,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>58</v>
       </c>
@@ -1139,7 +1169,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>61</v>
       </c>
@@ -1163,7 +1193,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>63</v>
       </c>
@@ -1187,7 +1217,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>66</v>
       </c>
@@ -1211,7 +1241,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>68</v>
       </c>
@@ -1232,7 +1262,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>101</v>
       </c>
@@ -1250,28 +1280,28 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E22" s="3"/>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E23" s="3"/>
       <c r="F23" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E24" s="3"/>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1292,7 +1322,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>30</v>
@@ -1322,7 +1352,7 @@
         <v>41681</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>34</v>
@@ -1353,28 +1383,68 @@
         <v>41681</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="E28" s="3"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.105</v>
+      </c>
       <c r="F28" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="E29" s="3"/>
+        <v>1.05</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H28" t="s">
+        <v>121</v>
+      </c>
+      <c r="I28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.13</v>
+      </c>
       <c r="F29" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>1.04</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E30" s="3"/>
       <c r="F30" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1401,7 +1471,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>45</v>
       </c>
@@ -1417,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>46</v>
       </c>
@@ -1427,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>74</v>
       </c>
@@ -1448,14 +1518,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E35" s="3"/>
       <c r="F35" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1479,7 +1549,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>20</v>
       </c>
@@ -1503,14 +1573,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
         <v>116</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>107</v>
       </c>
@@ -1534,7 +1604,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
         <v>70</v>
       </c>
@@ -1555,7 +1625,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>71</v>
       </c>
@@ -1565,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="12" customFormat="1">
+    <row r="42" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="12" t="s">
         <v>77</v>
       </c>
@@ -1595,7 +1665,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>81</v>
       </c>
@@ -1625,7 +1695,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>95</v>
       </c>
@@ -1655,7 +1725,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B45" s="10" t="s">
         <v>109</v>
       </c>
@@ -1676,7 +1746,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B46" s="10" t="s">
         <v>110</v>
       </c>
@@ -1697,7 +1767,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>117</v>
       </c>
@@ -1706,31 +1776,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F48" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F49" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>22</v>
       </c>
       <c r="F51" s="3">
         <f>SUM(F5:F50)</f>
-        <v>2777.3399999999997</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>2779.43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>28</v>
       </c>
@@ -1739,19 +1809,19 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>27</v>
       </c>
       <c r="F55" s="3">
         <f>F51-F53</f>
-        <v>1612.3399999999997</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8">
+        <v>1614.4299999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>72</v>
       </c>
@@ -1775,7 +1845,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="2:8">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>72</v>
       </c>
@@ -1807,6 +1877,8 @@
     <hyperlink ref="G67" r:id="rId3"/>
     <hyperlink ref="G5" r:id="rId4"/>
     <hyperlink ref="C45" r:id="rId5"/>
+    <hyperlink ref="G28" r:id="rId6"/>
+    <hyperlink ref="G29" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1823,7 +1895,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1840,7 +1912,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Update human sensing parts
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -893,7 +893,7 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1391,14 +1391,14 @@
         <v>119</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E28" s="3">
-        <v>0.105</v>
+        <v>6.7199999999999996E-2</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="0"/>
-        <v>1.05</v>
+        <v>3.36</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>120</v>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="F51" s="3">
         <f>SUM(F5:F50)</f>
-        <v>2779.43</v>
+        <v>2781.74</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="F55" s="3">
         <f>F51-F53</f>
-        <v>1614.4299999999998</v>
+        <v>1616.7399999999998</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added headers for XBee
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="129">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -399,6 +399,15 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>Headers for Xbee</t>
+  </si>
+  <si>
+    <t>NPPN101BFCN-RC</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/NPPN101BFCN-RC/S5751-10-ND/804812</t>
   </si>
 </sst>
 </file>
@@ -408,7 +417,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +472,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -526,7 +540,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -543,6 +557,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -885,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1775,10 +1790,25 @@
         <v>41689</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" ht="15">
+      <c r="B47" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1.018</v>
+      </c>
       <c r="F47" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10.18</v>
+      </c>
+      <c r="G47" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -1799,7 +1829,7 @@
       </c>
       <c r="F51" s="3">
         <f>SUM(F5:F50)</f>
-        <v>2780.5299999999997</v>
+        <v>2790.7099999999996</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1823,7 +1853,7 @@
       </c>
       <c r="F55" s="3">
         <f>F51-F53</f>
-        <v>1615.5299999999997</v>
+        <v>1625.7099999999996</v>
       </c>
     </row>
     <row r="66" spans="2:8">

</xml_diff>

<commit_message>
Added parts received and updated costs for those parts being ordered.
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="133">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -311,15 +311,9 @@
     <t>Through hole, tv, 500 mA max output supply</t>
   </si>
   <si>
-    <t>http://www.hobbyexpress.com/gemfan_11x4.7_reverse_carbon_filled_1041840_prd1.htm?pSearchQueryId=4684805</t>
-  </si>
-  <si>
     <t>Blades opposite direction</t>
   </si>
   <si>
-    <t>http://www.hobbyexpress.com/gemfan_11x4.7_normal_carbon_filled_1041839_prd1.htm?pSearchQueryId=4684805</t>
-  </si>
-  <si>
     <t>http://hobbyking.com/hobbyking/store/__26486__NTM_Prop_Drive_Series_35_36A_1800Kv_875w_US_Warehouse_.html</t>
   </si>
   <si>
@@ -419,10 +413,13 @@
     <t>100ft</t>
   </si>
   <si>
-    <t>Barrel power cables</t>
-  </si>
-  <si>
     <t>8 replacements</t>
+  </si>
+  <si>
+    <t>http://www.hobbyexpress.com/11x4.7_apc_slowflyer_prop_1260_prd1.htm?pSearchQueryId=4690948</t>
+  </si>
+  <si>
+    <t>http://www.hobbyexpress.com/slowprop_1036592_prd1.htm?pSearchQueryId=4690948</t>
   </si>
 </sst>
 </file>
@@ -523,13 +520,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="38">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -583,7 +584,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="38">
+  <cellStyles count="42">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -618,6 +619,10 @@
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -923,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -999,7 +1004,7 @@
         <v>135</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F38" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F37" si="0">D5*E5</f>
         <v>270</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -1268,7 +1273,7 @@
         <v>184.8</v>
       </c>
       <c r="G19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J19" s="4">
         <v>41684</v>
@@ -1285,32 +1290,38 @@
         <v>5</v>
       </c>
       <c r="E20" s="3">
-        <v>3</v>
+        <v>3.16</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>15.8</v>
       </c>
       <c r="G20" t="s">
-        <v>98</v>
+        <v>131</v>
+      </c>
+      <c r="J20" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="B21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E21" s="3">
-        <v>3</v>
+        <v>4.74</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>28.44</v>
       </c>
       <c r="G21" t="s">
-        <v>96</v>
+        <v>132</v>
+      </c>
+      <c r="J21" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1379,10 +1390,10 @@
         <v>30</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="J26" s="4">
-        <v>41681</v>
+        <v>123</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1410,18 +1421,18 @@
         <v>33</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="J27" s="4">
-        <v>41681</v>
+        <v>124</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="B28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D28">
         <v>50</v>
@@ -1434,13 +1445,13 @@
         <v>3.36</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J28" s="15">
         <v>41690</v>
@@ -1448,10 +1459,10 @@
     </row>
     <row r="29" spans="1:10">
       <c r="B29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D29">
         <v>10</v>
@@ -1464,13 +1475,13 @@
         <v>1.2</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J29" s="15">
         <v>41690</v>
@@ -1478,10 +1489,10 @@
     </row>
     <row r="30" spans="1:10">
       <c r="B30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C30" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1494,7 +1505,7 @@
         <v>14.99</v>
       </c>
       <c r="G30" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J30" s="15">
         <v>41690</v>
@@ -1547,8 +1558,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J33" s="4">
-        <v>41689</v>
+      <c r="J33" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1582,400 +1593,376 @@
         <v>72</v>
       </c>
       <c r="J35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="B36" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36">
-        <v>4</v>
-      </c>
-      <c r="E36" s="3">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="F36" s="3">
-        <f t="shared" si="0"/>
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="G36" t="s">
-        <v>119</v>
-      </c>
-      <c r="I36" t="s">
-        <v>126</v>
-      </c>
-      <c r="J36" s="4">
-        <v>41690</v>
-      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" t="s">
+      <c r="A37" t="s">
         <v>8</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B37" t="s">
         <v>18</v>
       </c>
-      <c r="D38">
+      <c r="D37">
         <v>2</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E37" s="3">
         <v>0</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F37" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G37" t="s">
         <v>22</v>
       </c>
+      <c r="J37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3">
+        <v>39.99</v>
+      </c>
+      <c r="F38" s="3">
+        <f>D38*E38</f>
+        <v>0</v>
+      </c>
       <c r="J38" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:10">
-      <c r="B39" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39" s="3">
-        <v>39.99</v>
-      </c>
-      <c r="F39" s="3">
-        <f>D39*E39</f>
-        <v>0</v>
-      </c>
-      <c r="J39" t="s">
-        <v>116</v>
-      </c>
+      <c r="C39" t="s">
+        <v>105</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:10">
+      <c r="B40" t="s">
+        <v>100</v>
+      </c>
       <c r="C40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40" s="3">
+        <v>29.99</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" ref="F40:F50" si="2">D40*E40</f>
+        <v>149.94999999999999</v>
+      </c>
+      <c r="G40" t="s">
+        <v>98</v>
+      </c>
+      <c r="J40" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="41" spans="1:10">
-      <c r="B41" t="s">
-        <v>102</v>
+      <c r="B41" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="C41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41" s="3">
+        <v>15</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="G41" t="s">
         <v>101</v>
       </c>
-      <c r="D41">
-        <v>5</v>
-      </c>
-      <c r="E41" s="3">
-        <v>29.99</v>
-      </c>
-      <c r="F41" s="3">
-        <f t="shared" ref="F41:F51" si="2">D41*E41</f>
-        <v>149.94999999999999</v>
-      </c>
-      <c r="G41" t="s">
-        <v>100</v>
-      </c>
-      <c r="J41" t="s">
-        <v>89</v>
+      <c r="J41" s="4">
+        <v>41690</v>
       </c>
     </row>
     <row r="42" spans="1:10">
-      <c r="B42" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" t="s">
-        <v>106</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" s="3">
-        <v>15</v>
-      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" s="3"/>
       <c r="F42" s="3">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="G42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="11" customFormat="1">
+      <c r="B43" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="11">
+        <v>2</v>
+      </c>
+      <c r="E43" s="12">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="F43" s="12">
+        <f>D43*E43</f>
+        <v>69.900000000000006</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J43" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="B44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44" s="3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F44" s="3">
+        <f>D44*E44</f>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G44" t="s">
+        <v>78</v>
+      </c>
+      <c r="H44" t="s">
+        <v>80</v>
+      </c>
+      <c r="I44" t="s">
+        <v>81</v>
+      </c>
+      <c r="J44" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1.46</v>
+      </c>
+      <c r="F45" s="3">
+        <f t="shared" si="2"/>
+        <v>14.6</v>
+      </c>
+      <c r="G45" t="s">
+        <v>93</v>
+      </c>
+      <c r="H45" t="s">
+        <v>94</v>
+      </c>
+      <c r="I45" t="s">
+        <v>95</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="B46" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" s="3">
+        <v>14.99</v>
+      </c>
+      <c r="F46" s="3">
+        <f t="shared" si="2"/>
+        <v>29.98</v>
+      </c>
+      <c r="G46" t="s">
+        <v>115</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="B47" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="J42" s="4">
+      <c r="C47" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47" s="3">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="F47" s="3">
+        <f>E47*D47</f>
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="G47" t="s">
+        <v>117</v>
+      </c>
+      <c r="J47" s="4">
         <v>41690</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
-      <c r="B43" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3">
+    <row r="48" spans="1:10" ht="15">
+      <c r="B48" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48">
+        <v>10</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1.018</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="2"/>
+        <v>10.18</v>
+      </c>
+      <c r="G48" t="s">
+        <v>122</v>
+      </c>
+      <c r="I48" t="s">
+        <v>130</v>
+      </c>
+      <c r="J48" s="15">
+        <v>41690</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="F49" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="11" customFormat="1">
-      <c r="B44" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D44" s="11">
-        <v>2</v>
-      </c>
-      <c r="E44" s="12">
-        <v>34.950000000000003</v>
-      </c>
-      <c r="F44" s="12">
-        <f>D44*E44</f>
-        <v>69.900000000000006</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I44" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J44" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="B45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45">
-        <v>2</v>
-      </c>
-      <c r="E45" s="3">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="F45" s="3">
-        <f>D45*E45</f>
-        <v>19.899999999999999</v>
-      </c>
-      <c r="G45" t="s">
-        <v>78</v>
-      </c>
-      <c r="H45" t="s">
-        <v>80</v>
-      </c>
-      <c r="I45" t="s">
-        <v>81</v>
-      </c>
-      <c r="J45" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="B46" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46">
-        <v>10</v>
-      </c>
-      <c r="E46" s="3">
-        <v>1.46</v>
-      </c>
-      <c r="F46" s="3">
-        <f t="shared" si="2"/>
-        <v>14.6</v>
-      </c>
-      <c r="G46" t="s">
-        <v>93</v>
-      </c>
-      <c r="H46" t="s">
-        <v>94</v>
-      </c>
-      <c r="I46" t="s">
-        <v>95</v>
-      </c>
-      <c r="J46" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="B47" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C47" t="s">
-        <v>118</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47" s="3">
-        <v>14.99</v>
-      </c>
-      <c r="F47" s="3">
-        <f t="shared" si="2"/>
-        <v>14.99</v>
-      </c>
-      <c r="G47" t="s">
-        <v>117</v>
-      </c>
-      <c r="J47" s="4">
-        <v>41689</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="B48" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D48">
-        <v>2</v>
-      </c>
-      <c r="E48" s="3">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="F48" s="3">
-        <f>E48*D48</f>
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="G48" t="s">
-        <v>119</v>
-      </c>
-      <c r="J48" s="4">
-        <v>41690</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="15">
-      <c r="B49" t="s">
-        <v>122</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49">
-        <v>10</v>
-      </c>
-      <c r="E49" s="3">
-        <v>1.018</v>
-      </c>
-      <c r="F49" s="3">
-        <f t="shared" si="2"/>
-        <v>10.18</v>
-      </c>
-      <c r="G49" t="s">
-        <v>124</v>
-      </c>
-      <c r="I49" t="s">
-        <v>133</v>
-      </c>
-      <c r="J49" s="15">
-        <v>41690</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:6">
       <c r="F50" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
-      <c r="F51" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" t="s">
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
         <v>21</v>
       </c>
-      <c r="F53" s="3">
-        <f>SUM(F5:F52)</f>
-        <v>2816.2899999999995</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55" t="s">
+      <c r="F52" s="3">
+        <f>SUM(F5:F51)</f>
+        <v>2856.4599999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
         <v>26</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F54" s="3">
         <f>SUM(F32)</f>
         <v>1165</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57" t="s">
+    <row r="55" spans="1:6">
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
         <v>25</v>
       </c>
-      <c r="F57" s="3">
-        <f>F53-F55</f>
-        <v>1651.2899999999995</v>
+      <c r="F56" s="3">
+        <f>F52-F54</f>
+        <v>1691.4599999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8">
+      <c r="B67" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" s="3">
+        <v>23.75</v>
+      </c>
+      <c r="F67" s="3">
+        <f>D67*E67</f>
+        <v>23.75</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H67" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="2:8">
       <c r="B68" t="s">
         <v>68</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>82</v>
+      <c r="C68" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68" s="3">
-        <v>23.75</v>
+        <v>13.78</v>
       </c>
       <c r="F68" s="3">
         <f>D68*E68</f>
-        <v>23.75</v>
+        <v>13.78</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H68" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8">
-      <c r="B69" t="s">
-        <v>68</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-      <c r="E69" s="3">
-        <v>13.78</v>
-      </c>
-      <c r="F69" s="3">
-        <f>D69*E69</f>
-        <v>13.78</v>
-      </c>
-      <c r="G69" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H69" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1983,10 +1970,10 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G27" r:id="rId1"/>
-    <hyperlink ref="G68" r:id="rId2" location="dl"/>
-    <hyperlink ref="G69" r:id="rId3"/>
+    <hyperlink ref="G67" r:id="rId2" location="dl"/>
+    <hyperlink ref="G68" r:id="rId3"/>
     <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="C47" r:id="rId5" display="5V 3A BEC Step-Down Voltage Regulator"/>
+    <hyperlink ref="C46" r:id="rId5" display="5V 3A BEC Step-Down Voltage Regulator"/>
     <hyperlink ref="G28" r:id="rId6"/>
     <hyperlink ref="G29" r:id="rId7"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Added 5 point tamper proof bits
Added 5 point tamper proof bits
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="135">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -420,6 +420,12 @@
   </si>
   <si>
     <t>http://www.hobbyexpress.com/slowprop_1036592_prd1.htm?pSearchQueryId=4690948</t>
+  </si>
+  <si>
+    <t>5 point tool set for kinect</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/5-Point-TORX-Tamper-Proof-Bit-Set/dp/B007SOODHC/ref=sr_1_2?ie=UTF8&amp;qid=1392914223&amp;sr=8-2&amp;keywords=five+point+tamper+proof</t>
   </si>
 </sst>
 </file>
@@ -930,28 +936,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="28">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -983,11 +989,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1017,7 +1023,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>37</v>
       </c>
@@ -1041,7 +1047,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -1056,28 +1062,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1087,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>44</v>
       </c>
@@ -1111,7 +1117,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>44</v>
       </c>
@@ -1135,7 +1141,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>49</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>52</v>
       </c>
@@ -1183,7 +1189,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>54</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>57</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>59</v>
       </c>
@@ -1255,7 +1261,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>62</v>
       </c>
@@ -1279,7 +1285,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>64</v>
       </c>
@@ -1303,7 +1309,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>96</v>
       </c>
@@ -1324,28 +1330,39 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
-      <c r="E22" s="3"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>6.98</v>
+      </c>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>6.98</v>
+      </c>
+      <c r="G22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>
       <c r="F23" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1366,7 +1383,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>28</v>
@@ -1396,7 +1413,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>31</v>
@@ -1427,7 +1444,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>106</v>
       </c>
@@ -1457,7 +1474,7 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>110</v>
       </c>
@@ -1487,7 +1504,7 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>128</v>
       </c>
@@ -1511,12 +1528,12 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="J31" s="15"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1543,7 +1560,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>41</v>
       </c>
@@ -1562,7 +1579,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>42</v>
       </c>
@@ -1572,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>70</v>
       </c>
@@ -1596,12 +1613,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1625,7 +1642,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>20</v>
       </c>
@@ -1643,14 +1660,14 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>105</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>100</v>
       </c>
@@ -1674,7 +1691,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
         <v>66</v>
       </c>
@@ -1698,7 +1715,7 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>67</v>
       </c>
@@ -1708,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="11" customFormat="1">
+    <row r="43" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
         <v>73</v>
       </c>
@@ -1738,7 +1755,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>77</v>
       </c>
@@ -1768,7 +1785,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>91</v>
       </c>
@@ -1798,7 +1815,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
         <v>102</v>
       </c>
@@ -1822,7 +1839,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
         <v>103</v>
       </c>
@@ -1846,7 +1863,7 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15">
+    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>120</v>
       </c>
@@ -1873,31 +1890,31 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F49" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F50" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>21</v>
       </c>
       <c r="F52" s="3">
         <f>SUM(F5:F51)</f>
-        <v>2856.4599999999996</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>2863.4399999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -1906,19 +1923,19 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>25</v>
       </c>
       <c r="F56" s="3">
         <f>F52-F54</f>
-        <v>1691.4599999999996</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8">
+        <v>1698.4399999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>68</v>
       </c>
@@ -1942,7 +1959,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="2:8">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>68</v>
       </c>
@@ -1993,7 +2010,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2010,7 +2027,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Add IR sensor equipment
Multiplexer and adaptors
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="144">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -426,6 +426,33 @@
   </si>
   <si>
     <t>http://www.amazon.com/5-Point-TORX-Tamper-Proof-Bit-Set/dp/B007SOODHC/ref=sr_1_2?ie=UTF8&amp;qid=1392914223&amp;sr=8-2&amp;keywords=five+point+tamper+proof</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/PCA9547D,112/568-3380-5-ND/1125693</t>
+  </si>
+  <si>
+    <t>Allows for multiple Irs w/ one Arduino</t>
+  </si>
+  <si>
+    <t>Ordered: 1 + 3 replacements</t>
+  </si>
+  <si>
+    <t>i2C Multiplexer</t>
+  </si>
+  <si>
+    <t>PCA9547D</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?mpart=24-350000-10&amp;vendor=43</t>
+  </si>
+  <si>
+    <t>Adaptor for multiplexer</t>
+  </si>
+  <si>
+    <t>SOIC/DIP 24 pin adaptor</t>
+  </si>
+  <si>
+    <t>24-350000-10</t>
   </si>
 </sst>
 </file>
@@ -934,25 +961,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="3" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -989,11 +1016,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1010,7 +1037,7 @@
         <v>135</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F37" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F39" si="0">D5*E5</f>
         <v>270</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -1023,7 +1050,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>37</v>
       </c>
@@ -1047,7 +1074,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -1062,28 +1089,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1093,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>44</v>
       </c>
@@ -1117,7 +1144,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>44</v>
       </c>
@@ -1141,7 +1168,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>49</v>
       </c>
@@ -1165,7 +1192,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>52</v>
       </c>
@@ -1189,7 +1216,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>54</v>
       </c>
@@ -1213,7 +1240,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>57</v>
       </c>
@@ -1237,7 +1264,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>59</v>
       </c>
@@ -1261,7 +1288,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>62</v>
       </c>
@@ -1285,7 +1312,7 @@
         <v>41684</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>64</v>
       </c>
@@ -1309,7 +1336,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>96</v>
       </c>
@@ -1330,7 +1357,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>133</v>
       </c>
@@ -1348,21 +1375,21 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>
       <c r="F23" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1383,7 +1410,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>28</v>
@@ -1413,7 +1440,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>31</v>
@@ -1444,7 +1471,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>106</v>
       </c>
@@ -1474,7 +1501,7 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>110</v>
       </c>
@@ -1504,7 +1531,7 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>128</v>
       </c>
@@ -1528,458 +1555,514 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2.42</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="0"/>
+        <v>9.68</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H31" t="s">
+        <v>136</v>
+      </c>
+      <c r="I31" t="s">
+        <v>137</v>
+      </c>
       <c r="J31" s="15"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>143</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E32" s="3">
-        <v>1165</v>
+        <v>8.42</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="0"/>
+        <v>33.68</v>
+      </c>
+      <c r="G32" t="s">
+        <v>140</v>
+      </c>
+      <c r="H32" t="s">
+        <v>141</v>
+      </c>
+      <c r="I32" t="s">
+        <v>137</v>
+      </c>
+      <c r="J32" s="15"/>
+    </row>
+    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3">
         <v>1165</v>
       </c>
-      <c r="G32" t="s">
+      <c r="F34" s="3">
+        <f t="shared" si="0"/>
+        <v>1165</v>
+      </c>
+      <c r="G34" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J34" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>41</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>40</v>
       </c>
-      <c r="D33">
+      <c r="D35">
         <v>2</v>
       </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3">
+      <c r="E35" s="3"/>
+      <c r="F35" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J35" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3">
+      <c r="E36" s="3"/>
+      <c r="F36" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>70</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>71</v>
       </c>
-      <c r="D35">
+      <c r="D37">
         <v>1</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E37" s="3">
         <v>39</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F37" s="3">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G37" t="s">
         <v>72</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>8</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>18</v>
       </c>
-      <c r="D37">
+      <c r="D39">
         <v>2</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E39" s="3">
         <v>0</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F39" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G39" t="s">
         <v>22</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J39" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
         <v>20</v>
       </c>
-      <c r="D38">
+      <c r="D40">
         <v>0</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E40" s="3">
         <v>39.99</v>
       </c>
-      <c r="F38" s="3">
-        <f>D38*E38</f>
+      <c r="F40" s="3">
+        <f>D40*E40</f>
         <v>0</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J40" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
         <v>105</v>
       </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>100</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>99</v>
       </c>
-      <c r="D40">
+      <c r="D42">
         <v>5</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E42" s="3">
         <v>29.99</v>
       </c>
-      <c r="F40" s="3">
-        <f t="shared" ref="F40:F50" si="2">D40*E40</f>
+      <c r="F42" s="3">
+        <f t="shared" ref="F42:F52" si="2">D42*E42</f>
         <v>149.94999999999999</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G42" t="s">
         <v>98</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J42" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="10" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>104</v>
       </c>
-      <c r="D41">
+      <c r="D43">
         <v>2</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E43" s="3">
         <v>15</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F43" s="3">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G43" t="s">
         <v>101</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J43" s="4">
         <v>41690</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3">
+      <c r="E44" s="3"/>
+      <c r="F44" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
+    <row r="45" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C45" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D45" s="11">
         <v>2</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E45" s="12">
         <v>34.950000000000003</v>
       </c>
-      <c r="F43" s="12">
-        <f>D43*E43</f>
+      <c r="F45" s="12">
+        <f>D45*E45</f>
         <v>69.900000000000006</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="G45" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="H45" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I43" s="11" t="s">
+      <c r="I45" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="J43" s="13" t="s">
+      <c r="J45" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
         <v>77</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>79</v>
       </c>
-      <c r="D44">
+      <c r="D46">
         <v>2</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E46" s="3">
         <v>9.9499999999999993</v>
       </c>
-      <c r="F44" s="3">
-        <f>D44*E44</f>
+      <c r="F46" s="3">
+        <f>D46*E46</f>
         <v>19.899999999999999</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G46" t="s">
         <v>78</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H46" t="s">
         <v>80</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I46" t="s">
         <v>81</v>
       </c>
-      <c r="J44" s="13" t="s">
+      <c r="J46" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C47" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D45">
+      <c r="D47">
         <v>10</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E47" s="3">
         <v>1.46</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F47" s="3">
         <f t="shared" si="2"/>
         <v>14.6</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G47" t="s">
         <v>93</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H47" t="s">
         <v>94</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I47" t="s">
         <v>95</v>
       </c>
-      <c r="J45" s="13" t="s">
+      <c r="J47" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="10" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B48" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C48" t="s">
         <v>116</v>
       </c>
-      <c r="D46">
+      <c r="D48">
         <v>2</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E48" s="3">
         <v>14.99</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F48" s="3">
         <f t="shared" si="2"/>
         <v>29.98</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G48" t="s">
         <v>115</v>
       </c>
-      <c r="J46" s="4" t="s">
+      <c r="J48" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="10" t="s">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B49" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C49" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D47">
+      <c r="D49">
         <v>4</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E49" s="3">
         <v>2.0299999999999998</v>
       </c>
-      <c r="F47" s="3">
-        <f>E47*D47</f>
+      <c r="F49" s="3">
+        <f>E49*D49</f>
         <v>8.1199999999999992</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G49" t="s">
         <v>117</v>
       </c>
-      <c r="J47" s="4">
+      <c r="J49" s="4">
         <v>41690</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="50" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C50" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="D48">
+      <c r="D50">
         <v>10</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E50" s="3">
         <v>1.018</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F50" s="3">
         <f t="shared" si="2"/>
         <v>10.18</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G50" t="s">
         <v>122</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I50" t="s">
         <v>130</v>
       </c>
-      <c r="J48" s="15">
+      <c r="J50" s="15">
         <v>41690</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="3">
+    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="F51" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F50" s="3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F52" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>21</v>
       </c>
-      <c r="F52" s="3">
-        <f>SUM(F5:F51)</f>
-        <v>2863.4399999999996</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="F54" s="3">
+        <f>SUM(F5:F53)</f>
+        <v>2906.7999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>26</v>
       </c>
-      <c r="F54" s="3">
-        <f>SUM(F32)</f>
+      <c r="F56" s="3">
+        <f>SUM(F34)</f>
         <v>1165</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="3">
-        <f>F52-F54</f>
-        <v>1698.4399999999996</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+      <c r="F58" s="3">
+        <f>F54-F56</f>
+        <v>1741.7999999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
         <v>68</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C69" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D67">
+      <c r="D69">
         <v>1</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E69" s="3">
         <v>23.75</v>
       </c>
-      <c r="F67" s="3">
-        <f>D67*E67</f>
+      <c r="F69" s="3">
+        <f>D69*E69</f>
         <v>23.75</v>
       </c>
-      <c r="G67" s="7" t="s">
+      <c r="G69" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H69" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
         <v>68</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C70" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D68">
+      <c r="D70">
         <v>1</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E70" s="3">
         <v>13.78</v>
       </c>
-      <c r="F68" s="3">
-        <f>D68*E68</f>
+      <c r="F70" s="3">
+        <f>D70*E70</f>
         <v>13.78</v>
       </c>
-      <c r="G68" s="7" t="s">
+      <c r="G70" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H70" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1987,12 +2070,13 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G27" r:id="rId1"/>
-    <hyperlink ref="G67" r:id="rId2" location="dl"/>
-    <hyperlink ref="G68" r:id="rId3"/>
+    <hyperlink ref="G69" r:id="rId2" location="dl"/>
+    <hyperlink ref="G70" r:id="rId3"/>
     <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="C46" r:id="rId5" display="5V 3A BEC Step-Down Voltage Regulator"/>
+    <hyperlink ref="C48" r:id="rId5" display="5V 3A BEC Step-Down Voltage Regulator"/>
     <hyperlink ref="G28" r:id="rId6"/>
     <hyperlink ref="G29" r:id="rId7"/>
+    <hyperlink ref="G31" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2010,7 +2094,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2027,7 +2111,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Added Power Module, Wires, Connectors
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="158">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -450,6 +450,51 @@
   </si>
   <si>
     <t>In house</t>
+  </si>
+  <si>
+    <t>Power Module</t>
+  </si>
+  <si>
+    <t>https://store.3drobotics.com/products/apm-power-module-with-xt60-connectors</t>
+  </si>
+  <si>
+    <t>APM Power Module</t>
+  </si>
+  <si>
+    <t>http://hobbyking.com/hobbyking/store/__42755__Turnigy_Pure_Silicone_Wire_16AWG_1mtr_BLACK_USA_warehouse_.html</t>
+  </si>
+  <si>
+    <t>B16A483-06</t>
+  </si>
+  <si>
+    <t>16 AWG wire</t>
+  </si>
+  <si>
+    <t>http://hobbyking.com/hobbyking/store/__42536__3_5mm_3_wire_Bullet_connector_for_motor_5pairs_bag_USA_warehouse_.html</t>
+  </si>
+  <si>
+    <t>9001-AB</t>
+  </si>
+  <si>
+    <t>Set of 3.5mm bullet connectors</t>
+  </si>
+  <si>
+    <t>https://store.3drobotics.com/products/deans-ultra-plug-connector-male</t>
+  </si>
+  <si>
+    <t>Deans Ultra Plug Connector MALE</t>
+  </si>
+  <si>
+    <t>Deans Male</t>
+  </si>
+  <si>
+    <t>Deans Female</t>
+  </si>
+  <si>
+    <t>https://store.3drobotics.com/products/deans-ultra-plug-connector-female</t>
+  </si>
+  <si>
+    <t>Deans Ultra Plug Connector FEMALE</t>
   </si>
 </sst>
 </file>
@@ -515,16 +560,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="4">
@@ -556,13 +601,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -617,11 +664,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -660,6 +707,8 @@
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -965,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1483,7 +1532,7 @@
       <c r="I27" t="s">
         <v>125</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="J27" s="14" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1513,7 +1562,7 @@
       <c r="I28" t="s">
         <v>126</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="J28" s="14" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1537,7 +1586,7 @@
       <c r="G29" t="s">
         <v>127</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="J29" s="14" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1567,7 +1616,7 @@
       <c r="I30" t="s">
         <v>135</v>
       </c>
-      <c r="J30" s="15">
+      <c r="J30" s="14">
         <v>41695</v>
       </c>
     </row>
@@ -1597,14 +1646,14 @@
       <c r="I31" t="s">
         <v>135</v>
       </c>
-      <c r="J31" s="15">
+      <c r="J31" s="14">
         <v>41330</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="J32" s="15"/>
+      <c r="J32" s="14"/>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
@@ -1754,7 +1803,7 @@
         <v>29.99</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" ref="F41:F51" si="2">D41*E41</f>
+        <f t="shared" ref="F41:F54" si="2">D41*E41</f>
         <v>149.94999999999999</v>
       </c>
       <c r="G41" t="s">
@@ -1889,7 +1938,7 @@
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="15" t="s">
         <v>102</v>
       </c>
       <c r="C47" t="s">
@@ -1913,10 +1962,10 @@
       </c>
     </row>
     <row r="48" spans="1:10">
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" t="s">
         <v>118</v>
       </c>
       <c r="D48">
@@ -1936,11 +1985,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15">
+    <row r="49" spans="1:10">
       <c r="B49" t="s">
         <v>120</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" t="s">
         <v>121</v>
       </c>
       <c r="D49">
@@ -1959,100 +2008,193 @@
       <c r="I49" t="s">
         <v>130</v>
       </c>
-      <c r="J49" s="15" t="s">
+      <c r="J49" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:10">
+      <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" s="3">
+        <v>24.99</v>
+      </c>
       <c r="F50" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>24.99</v>
+      </c>
+      <c r="G50" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:10">
+      <c r="B51" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" t="s">
+        <v>157</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
       <c r="F51" s="3">
+        <f>E51*D51</f>
+        <v>6</v>
+      </c>
+      <c r="G51" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="B52" t="s">
+        <v>154</v>
+      </c>
+      <c r="C52" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52">
+        <v>6</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <f>E52*D52</f>
+        <v>6</v>
+      </c>
+      <c r="G52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15">
+      <c r="B53" t="s">
+        <v>151</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" s="3">
+        <v>5.07</v>
+      </c>
+      <c r="F53" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" t="s">
-        <v>21</v>
-      </c>
-      <c r="F53" s="3">
-        <f>SUM(F5:F52)</f>
-        <v>2884.8299999999995</v>
+        <v>5.07</v>
+      </c>
+      <c r="G53" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:10">
-      <c r="F54" s="3"/>
+      <c r="B54" t="s">
+        <v>148</v>
+      </c>
+      <c r="C54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54">
+        <v>4</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1.36</v>
+      </c>
+      <c r="F54" s="3">
+        <f t="shared" si="2"/>
+        <v>5.44</v>
+      </c>
+      <c r="G54" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="F55" s="3">
+        <f>SUM(F5:F54)</f>
+        <v>2932.3299999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
         <v>26</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F57" s="3">
         <f>SUM(F33)</f>
         <v>1165</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57" t="s">
+    <row r="58" spans="1:10">
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" t="s">
         <v>25</v>
       </c>
-      <c r="F57" s="3">
-        <f>F53-F55</f>
-        <v>1719.8299999999995</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8">
-      <c r="B68" t="s">
+      <c r="F59" s="3">
+        <f>F55-F57</f>
+        <v>1767.3299999999995</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8">
+      <c r="B70" t="s">
         <v>68</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C70" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D68">
+      <c r="D70">
         <v>1</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E70" s="3">
         <v>23.75</v>
       </c>
-      <c r="F68" s="3">
-        <f>D68*E68</f>
+      <c r="F70" s="3">
+        <f>D70*E70</f>
         <v>23.75</v>
       </c>
-      <c r="G68" s="7" t="s">
+      <c r="G70" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="2:8">
-      <c r="B69" t="s">
+    <row r="71" spans="2:8">
+      <c r="B71" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C71" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D69">
+      <c r="D71">
         <v>1</v>
       </c>
-      <c r="E69" s="3">
+      <c r="E71" s="3">
         <v>13.78</v>
       </c>
-      <c r="F69" s="3">
-        <f>D69*E69</f>
+      <c r="F71" s="3">
+        <f>D71*E71</f>
         <v>13.78</v>
       </c>
-      <c r="G69" s="7" t="s">
+      <c r="G71" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H71" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2060,8 +2202,8 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G26" r:id="rId1"/>
-    <hyperlink ref="G68" r:id="rId2" location="dl"/>
-    <hyperlink ref="G69" r:id="rId3"/>
+    <hyperlink ref="G70" r:id="rId2" location="dl"/>
+    <hyperlink ref="G71" r:id="rId3"/>
     <hyperlink ref="G5" r:id="rId4"/>
     <hyperlink ref="C47" r:id="rId5" display="5V 3A BEC Step-Down Voltage Regulator"/>
     <hyperlink ref="G27" r:id="rId6"/>
@@ -2069,6 +2211,7 @@
     <hyperlink ref="G30" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added landing gear extensions
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="163">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -504,6 +504,12 @@
   </si>
   <si>
     <t>GON-D4T6</t>
+  </si>
+  <si>
+    <t>Landing Gear Extentions</t>
+  </si>
+  <si>
+    <t>http://www.hobbyking.com/hobbyking/store/__28221__Extended_Landing_Skid_Set_for_SK450_Quadcopter_Frame.html</t>
   </si>
 </sst>
 </file>
@@ -581,11 +587,9 @@
       <name val="Verdana"/>
     </font>
     <font>
-      <b/>
       <sz val="13.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -696,10 +700,10 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="56">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1059,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1135,7 +1139,7 @@
         <v>135</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F38" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F39" si="0">D5*E5</f>
         <v>270</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -1447,7 +1451,7 @@
       <c r="B22" t="s">
         <v>158</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="18" t="s">
         <v>160</v>
       </c>
       <c r="D22">
@@ -1463,286 +1467,291 @@
       <c r="G22" t="s">
         <v>159</v>
       </c>
-      <c r="J22" s="18">
+      <c r="J22" s="17">
         <v>41710</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+    <row r="23" spans="1:10" ht="18">
+      <c r="B23" t="s">
+        <v>161</v>
+      </c>
+      <c r="C23" s="18">
+        <v>9171000151</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3">
+        <v>9.49</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="0"/>
+        <v>18.98</v>
+      </c>
+      <c r="G23" t="s">
+        <v>162</v>
+      </c>
+      <c r="J23" s="17">
+        <v>41710</v>
+      </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" t="s">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
         <v>6</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>17</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>1</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E25" s="3">
         <v>144.13999999999999</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F25" s="3">
         <f t="shared" si="0"/>
         <v>144.13999999999999</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J25" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="5">
-        <v>6</v>
-      </c>
-      <c r="E25" s="6">
-        <v>50</v>
-      </c>
-      <c r="F25" s="6">
-        <v>400</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D26" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E26" s="6">
-        <v>1.42</v>
+        <v>50</v>
       </c>
       <c r="F26" s="6">
-        <f>D26*E26</f>
-        <v>5.68</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>43</v>
+        <v>400</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="B27" t="s">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="5">
+        <v>4</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1.42</v>
+      </c>
+      <c r="F27" s="6">
+        <f>D27*E27</f>
+        <v>5.68</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="B28" t="s">
         <v>106</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>107</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>50</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E28" s="3">
         <v>6.7199999999999996E-2</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F28" s="3">
         <f t="shared" si="0"/>
         <v>3.36</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G28" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H28" t="s">
         <v>109</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I28" t="s">
         <v>125</v>
       </c>
-      <c r="J27" s="14" t="s">
+      <c r="J28" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="B28" t="s">
+    <row r="29" spans="1:10">
+      <c r="B29" t="s">
         <v>110</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>111</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>10</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E29" s="3">
         <v>0.12</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F29" s="3">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H29" t="s">
         <v>113</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I29" t="s">
         <v>126</v>
       </c>
-      <c r="J28" s="14" t="s">
+      <c r="J29" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
-      <c r="B29" t="s">
+    <row r="30" spans="1:10">
+      <c r="B30" t="s">
         <v>128</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>129</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>0</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E30" s="3">
         <v>14.99</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F30" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" t="s">
         <v>127</v>
       </c>
-      <c r="J29" s="14" t="s">
+      <c r="J30" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
-      <c r="B30" t="s">
+    <row r="31" spans="1:10">
+      <c r="B31" t="s">
         <v>136</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>137</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>4</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E31" s="3">
         <v>2.42</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F31" s="3">
         <f t="shared" si="0"/>
         <v>9.68</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G31" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>134</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I31" t="s">
         <v>135</v>
       </c>
-      <c r="J30" s="14">
+      <c r="J31" s="14">
         <v>41695</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
-      <c r="B31" t="s">
+    <row r="32" spans="1:10">
+      <c r="B32" t="s">
         <v>140</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>141</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>4</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E32" s="3">
         <v>8.42</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F32" s="3">
         <f t="shared" si="0"/>
         <v>33.68</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G32" t="s">
         <v>138</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H32" t="s">
         <v>139</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I32" t="s">
         <v>135</v>
       </c>
-      <c r="J31" s="14">
+      <c r="J32" s="14">
         <v>41330</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="J32" s="14"/>
-    </row>
     <row r="33" spans="1:10">
-      <c r="A33" t="s">
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
         <v>7</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>16</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>23</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <v>1</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E34" s="3">
         <v>1165</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F34" s="3">
         <f t="shared" si="0"/>
         <v>1165</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G34" t="s">
         <v>24</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="B34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>89</v>
@@ -1750,205 +1759,194 @@
     </row>
     <row r="35" spans="1:10">
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J35" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="36" spans="1:10">
       <c r="B36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" t="s">
-        <v>71</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" s="3">
-        <v>39</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E36" s="3"/>
       <c r="F36" s="3">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3">
         <v>39</v>
       </c>
-      <c r="G36" t="s">
+      <c r="F37" s="3">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="G37" t="s">
         <v>72</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="J37" s="4"/>
-    </row>
     <row r="38" spans="1:10">
-      <c r="A38" t="s">
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" t="s">
         <v>8</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>18</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>2</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E39" s="3">
         <v>0</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F39" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G39" t="s">
         <v>22</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J39" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
-      <c r="B39" t="s">
+    <row r="40" spans="1:10">
+      <c r="B40" t="s">
         <v>20</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>0</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E40" s="3">
         <v>39.99</v>
       </c>
-      <c r="F39" s="3">
-        <f>D39*E39</f>
+      <c r="F40" s="3">
+        <f>D40*E40</f>
         <v>0</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J40" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
-      <c r="C40" t="s">
+    <row r="41" spans="1:10">
+      <c r="C41" t="s">
         <v>105</v>
       </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="B41" t="s">
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="B42" t="s">
         <v>100</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>99</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <v>5</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E42" s="3">
         <v>29.99</v>
       </c>
-      <c r="F41" s="3">
-        <f t="shared" ref="F41:F54" si="2">D41*E41</f>
+      <c r="F42" s="3">
+        <f t="shared" ref="F42:F55" si="2">D42*E42</f>
         <v>149.94999999999999</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G42" t="s">
         <v>98</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J42" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="B42" s="10" t="s">
+    <row r="43" spans="1:10">
+      <c r="B43" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>104</v>
       </c>
-      <c r="D42">
+      <c r="D43">
         <v>2</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E43" s="3">
         <v>15</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F43" s="3">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G43" t="s">
         <v>101</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J43" s="4">
         <v>41690</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
-      <c r="B43" t="s">
+    <row r="44" spans="1:10">
+      <c r="B44" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3">
+      <c r="E44" s="3"/>
+      <c r="F44" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="11" customFormat="1">
-      <c r="B44" s="11" t="s">
+    <row r="45" spans="1:10" s="11" customFormat="1">
+      <c r="B45" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C45" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D44" s="11">
+      <c r="D45" s="11">
         <v>2</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E45" s="12">
         <v>34.950000000000003</v>
       </c>
-      <c r="F44" s="12">
-        <f>D44*E44</f>
+      <c r="F45" s="12">
+        <f>D45*E45</f>
         <v>69.900000000000006</v>
       </c>
-      <c r="G44" s="11" t="s">
+      <c r="G45" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="H44" s="11" t="s">
+      <c r="H45" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I44" s="11" t="s">
+      <c r="I45" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="J44" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="B45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45">
-        <v>2</v>
-      </c>
-      <c r="E45" s="3">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="F45" s="3">
-        <f>D45*E45</f>
-        <v>19.899999999999999</v>
-      </c>
-      <c r="G45" t="s">
-        <v>78</v>
-      </c>
-      <c r="H45" t="s">
-        <v>80</v>
-      </c>
-      <c r="I45" t="s">
-        <v>81</v>
       </c>
       <c r="J45" s="13" t="s">
         <v>89</v>
@@ -1956,157 +1954,166 @@
     </row>
     <row r="46" spans="1:10">
       <c r="B46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" s="3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F46" s="3">
+        <f>D46*E46</f>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G46" t="s">
+        <v>78</v>
+      </c>
+      <c r="H46" t="s">
+        <v>80</v>
+      </c>
+      <c r="I46" t="s">
+        <v>81</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="B47" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C47" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <v>10</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E47" s="3">
         <v>1.46</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F47" s="3">
         <f t="shared" si="2"/>
         <v>14.6</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G47" t="s">
         <v>93</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H47" t="s">
         <v>94</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I47" t="s">
         <v>95</v>
       </c>
-      <c r="J46" s="13" t="s">
+      <c r="J47" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
-      <c r="B47" s="15" t="s">
+    <row r="48" spans="1:10">
+      <c r="B48" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>116</v>
       </c>
-      <c r="D47">
+      <c r="D48">
         <v>2</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E48" s="3">
         <v>14.99</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F48" s="3">
         <f t="shared" si="2"/>
         <v>29.98</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G48" t="s">
         <v>115</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="B48" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" t="s">
-        <v>118</v>
-      </c>
-      <c r="D48">
-        <v>4</v>
-      </c>
-      <c r="E48" s="3">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="F48" s="3">
-        <f>E48*D48</f>
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="G48" t="s">
-        <v>117</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:10">
-      <c r="B49" t="s">
+      <c r="B49" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="E49" s="3">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="F49" s="3">
+        <f>E49*D49</f>
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="G49" t="s">
+        <v>117</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="B50" t="s">
         <v>120</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>121</v>
       </c>
-      <c r="D49">
+      <c r="D50">
         <v>10</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E50" s="3">
         <v>1.018</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F50" s="3">
         <f t="shared" si="2"/>
         <v>10.18</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G50" t="s">
         <v>122</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I50" t="s">
         <v>130</v>
       </c>
-      <c r="J49" s="14" t="s">
+      <c r="J50" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
-      <c r="B50" t="s">
+    <row r="51" spans="1:10">
+      <c r="B51" t="s">
         <v>143</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>145</v>
       </c>
-      <c r="D50">
+      <c r="D51">
         <v>1</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E51" s="3">
         <v>24.99</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F51" s="3">
         <f t="shared" si="2"/>
         <v>24.99</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G51" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="B51" t="s">
-        <v>155</v>
-      </c>
-      <c r="C51" t="s">
-        <v>157</v>
-      </c>
-      <c r="D51">
-        <v>6</v>
-      </c>
-      <c r="E51" s="3">
-        <v>1</v>
-      </c>
-      <c r="F51" s="3">
-        <f>E51*D51</f>
-        <v>6</v>
-      </c>
-      <c r="G51" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="B52" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C52" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D52">
         <v>6</v>
@@ -2119,152 +2126,172 @@
         <v>6</v>
       </c>
       <c r="G52" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="B53" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53">
+        <v>6</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3">
+        <f>E53*D53</f>
+        <v>6</v>
+      </c>
+      <c r="G53" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15">
-      <c r="B53" t="s">
+    <row r="54" spans="1:10" ht="15">
+      <c r="B54" t="s">
         <v>151</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="C54" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>1</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E54" s="3">
         <v>5.07</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F54" s="3">
         <f t="shared" si="2"/>
         <v>5.07</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>149</v>
       </c>
-      <c r="J53" s="18">
+      <c r="J54" s="17">
         <v>41710</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
-      <c r="B54" t="s">
+    <row r="55" spans="1:10">
+      <c r="B55" t="s">
         <v>148</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>147</v>
       </c>
-      <c r="D54">
+      <c r="D55">
         <v>4</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E55" s="3">
         <v>1.36</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F55" s="3">
         <f t="shared" si="2"/>
         <v>5.44</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G55" t="s">
         <v>146</v>
       </c>
-      <c r="J54" s="18">
+      <c r="J55" s="17">
         <v>41710</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
-      <c r="A55" t="s">
+    <row r="56" spans="1:10">
+      <c r="A56" t="s">
         <v>21</v>
       </c>
-      <c r="F55" s="3">
-        <f>SUM(F5:F54)</f>
-        <v>2946.53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="F56" s="3"/>
+      <c r="F56" s="3">
+        <f>SUM(F5:F55)</f>
+        <v>2965.5099999999998</v>
+      </c>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" t="s">
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" t="s">
         <v>26</v>
       </c>
-      <c r="F57" s="3">
-        <f>SUM(F33)</f>
+      <c r="F58" s="3">
+        <f>SUM(F34)</f>
         <v>1165</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
-      <c r="F58" s="3"/>
-    </row>
     <row r="59" spans="1:10">
-      <c r="A59" t="s">
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" t="s">
         <v>25</v>
       </c>
-      <c r="F59" s="3">
-        <f>F55-F57</f>
-        <v>1781.5300000000002</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8">
-      <c r="B70" t="s">
-        <v>68</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="E70" s="3">
-        <v>23.75</v>
-      </c>
-      <c r="F70" s="3">
-        <f>D70*E70</f>
-        <v>23.75</v>
-      </c>
-      <c r="G70" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H70" t="s">
-        <v>69</v>
+      <c r="F60" s="3">
+        <f>F56-F58</f>
+        <v>1800.5099999999998</v>
       </c>
     </row>
     <row r="71" spans="2:8">
       <c r="B71" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="8" t="s">
-        <v>85</v>
+      <c r="C71" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71" s="3">
-        <v>13.78</v>
+        <v>23.75</v>
       </c>
       <c r="F71" s="3">
         <f>D71*E71</f>
+        <v>23.75</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8">
+      <c r="B72" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72" s="3">
         <v>13.78</v>
       </c>
-      <c r="G71" s="7" t="s">
+      <c r="F72" s="3">
+        <f>D72*E72</f>
+        <v>13.78</v>
+      </c>
+      <c r="G72" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H72" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G26" r:id="rId1"/>
-    <hyperlink ref="G70" r:id="rId2" location="dl"/>
-    <hyperlink ref="G71" r:id="rId3"/>
+    <hyperlink ref="G27" r:id="rId1"/>
+    <hyperlink ref="G71" r:id="rId2" location="dl"/>
+    <hyperlink ref="G72" r:id="rId3"/>
     <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="C47" r:id="rId5" display="5V 3A BEC Step-Down Voltage Regulator"/>
-    <hyperlink ref="G27" r:id="rId6"/>
-    <hyperlink ref="G28" r:id="rId7"/>
-    <hyperlink ref="G30" r:id="rId8"/>
+    <hyperlink ref="C48" r:id="rId5" display="5V 3A BEC Step-Down Voltage Regulator"/>
+    <hyperlink ref="G28" r:id="rId6"/>
+    <hyperlink ref="G29" r:id="rId7"/>
+    <hyperlink ref="G31" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Fixed a couple of things, including automatic calculations
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" activeTab="1"/>
   </bookViews>
@@ -10,7 +10,7 @@
     <sheet name="Parts Purchased" sheetId="1" r:id="rId1"/>
     <sheet name="Parts in Use" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="238">
   <si>
     <t>UAV Equipment List</t>
   </si>
@@ -725,6 +725,15 @@
   </si>
   <si>
     <t>lsf_top</t>
+  </si>
+  <si>
+    <t>18-8 Stainless Steel Button-Head Socket Cap Screw, M3 Size, 18 mm Long, 0.5 mm Pitch, packs of 100</t>
+  </si>
+  <si>
+    <t>92095A472</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#92095a472/=rncipl</t>
   </si>
 </sst>
 </file>
@@ -852,13 +861,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -948,7 +959,7 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1006,6 +1017,8 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -1311,30 +1324,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62:J63"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="28">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1366,11 +1379,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1387,7 +1400,7 @@
         <v>135</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F35" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F36" si="0">D5*E5</f>
         <v>270</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -1400,7 +1413,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="B6" t="s">
         <v>37</v>
       </c>
@@ -1424,7 +1437,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -1439,26 +1452,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="B12" t="s">
         <v>44</v>
       </c>
@@ -1482,7 +1495,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="B13" t="s">
         <v>44</v>
       </c>
@@ -1506,7 +1519,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="B14" t="s">
         <v>49</v>
       </c>
@@ -1530,7 +1543,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="B15" t="s">
         <v>52</v>
       </c>
@@ -1554,7 +1567,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="B16" t="s">
         <v>54</v>
       </c>
@@ -1578,7 +1591,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="B17" t="s">
         <v>57</v>
       </c>
@@ -1602,7 +1615,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="B18" t="s">
         <v>59</v>
       </c>
@@ -1626,7 +1639,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="B19" t="s">
         <v>62</v>
       </c>
@@ -1650,7 +1663,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="B20" t="s">
         <v>64</v>
       </c>
@@ -1674,7 +1687,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="B21" t="s">
         <v>96</v>
       </c>
@@ -1695,7 +1708,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="B22" t="s">
         <v>155</v>
       </c>
@@ -1715,11 +1728,11 @@
       <c r="G22" t="s">
         <v>156</v>
       </c>
-      <c r="J22" s="17">
-        <v>41710</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="B23" t="s">
         <v>158</v>
       </c>
@@ -1739,11 +1752,11 @@
       <c r="G23" t="s">
         <v>159</v>
       </c>
-      <c r="J23" s="17">
-        <v>41710</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="B24" s="18" t="s">
         <v>160</v>
       </c>
@@ -1762,7 +1775,7 @@
       </c>
       <c r="J24" s="17"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="B25" t="s">
         <v>161</v>
       </c>
@@ -1781,741 +1794,742 @@
       </c>
       <c r="J25" s="17"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="26" spans="1:10">
+      <c r="B26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" t="s">
+        <v>236</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
         <v>6</v>
       </c>
-      <c r="B27" t="s">
+      <c r="F26" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>237</v>
+      </c>
+      <c r="J26" s="17">
+        <v>41751</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="J27" s="17"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
         <v>17</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" s="3">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
         <v>144.13999999999999</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F28" s="3">
         <f t="shared" si="0"/>
         <v>144.13999999999999</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J28" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="5">
-        <v>6</v>
-      </c>
-      <c r="E28" s="6">
-        <v>50</v>
-      </c>
-      <c r="F28" s="6">
-        <v>400</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="5">
+        <v>6</v>
+      </c>
+      <c r="E29" s="6">
+        <v>50</v>
+      </c>
+      <c r="F29" s="6">
+        <v>400</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D30" s="5">
         <v>4</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E30" s="6">
         <v>1.42</v>
       </c>
-      <c r="F29" s="6">
-        <f>D29*E29</f>
+      <c r="F30" s="6">
+        <f>D30*E30</f>
         <v>5.68</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G30" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="J29" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="J30" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="B31" t="s">
         <v>105</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>106</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>50</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E31" s="3">
         <v>6.7199999999999996E-2</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F31" s="3">
         <f t="shared" si="0"/>
         <v>3.36</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G31" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>108</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I31" t="s">
         <v>122</v>
       </c>
-      <c r="J30" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="J31" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="B32" t="s">
         <v>109</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>110</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>10</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E32" s="3">
         <v>0.12</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F32" s="3">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G32" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H32" t="s">
         <v>112</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I32" t="s">
         <v>123</v>
       </c>
-      <c r="J31" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="J32" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="B33" t="s">
         <v>125</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>126</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <v>0</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E33" s="3">
         <v>14.99</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F33" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G33" t="s">
         <v>124</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="J33" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="34" spans="1:10">
+      <c r="B34" t="s">
         <v>133</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>134</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <v>4</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E34" s="3">
         <v>2.42</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F34" s="3">
         <f t="shared" si="0"/>
         <v>9.68</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G34" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" t="s">
         <v>131</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I34" t="s">
         <v>132</v>
       </c>
-      <c r="J33" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="J34" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="B35" t="s">
         <v>137</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>138</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <v>4</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E35" s="3">
         <v>8.42</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F35" s="3">
         <f t="shared" si="0"/>
         <v>33.68</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G35" t="s">
         <v>135</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H35" t="s">
         <v>136</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I35" t="s">
         <v>132</v>
       </c>
-      <c r="J34" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="20" t="s">
+      <c r="J35" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15">
+      <c r="B36" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" s="3">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3">
         <v>62.91</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F36" s="3">
         <f t="shared" si="0"/>
         <v>62.91</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G36" t="s">
         <v>208</v>
       </c>
-      <c r="J35" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="J36" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
         <v>7</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>16</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>23</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" s="3">
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3">
         <v>1165</v>
       </c>
-      <c r="F37" s="3">
-        <f t="shared" ref="F37:F42" si="2">D37*E37</f>
+      <c r="F38" s="3">
+        <f t="shared" ref="F38:F43" si="2">D38*E38</f>
         <v>1165</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G38" t="s">
         <v>24</v>
       </c>
-      <c r="J37" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="J38" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>40</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>2</v>
-      </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>42</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J39" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="B40" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" s="3">
-        <v>39</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E40" s="3"/>
       <c r="F40" s="3">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3">
         <v>39</v>
-      </c>
-      <c r="G40" t="s">
-        <v>72</v>
-      </c>
-      <c r="J40" s="4">
-        <v>41690</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>209</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" s="3">
-        <v>79.790000000000006</v>
       </c>
       <c r="F41" s="3">
         <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="G41" t="s">
+        <v>72</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="18">
+      <c r="B42" t="s">
+        <v>209</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
         <v>79.790000000000006</v>
-      </c>
-      <c r="G41" t="s">
-        <v>211</v>
-      </c>
-      <c r="J41" s="4">
-        <v>41744</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>212</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" s="3">
-        <v>6.13</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" si="2"/>
-        <v>6.13</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="G42" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="J42" s="4">
         <v>41744</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="43" spans="1:10" ht="18">
+      <c r="B43" t="s">
+        <v>212</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <v>6.13</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="2"/>
+        <v>6.13</v>
+      </c>
+      <c r="G43" t="s">
+        <v>214</v>
+      </c>
+      <c r="J43" s="4">
+        <v>41744</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" t="s">
         <v>8</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>18</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <v>2</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E46" s="3">
         <v>0</v>
-      </c>
-      <c r="F45" s="3">
-        <f>D45*E45</f>
-        <v>0</v>
-      </c>
-      <c r="G45" t="s">
-        <v>22</v>
-      </c>
-      <c r="J45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>215</v>
-      </c>
-      <c r="C46" t="s">
-        <v>216</v>
-      </c>
-      <c r="D46">
-        <v>4</v>
-      </c>
-      <c r="E46" s="3">
-        <v>169.99</v>
       </c>
       <c r="F46" s="3">
         <f>D46*E46</f>
-        <v>679.96</v>
+        <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>217</v>
-      </c>
-      <c r="H46" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J46" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="B47" t="s">
-        <v>218</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>219</v>
+        <v>215</v>
+      </c>
+      <c r="C47" t="s">
+        <v>216</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E47" s="3">
-        <v>89.99</v>
+        <v>169.99</v>
       </c>
       <c r="F47" s="3">
         <f>D47*E47</f>
+        <v>679.96</v>
+      </c>
+      <c r="G47" t="s">
+        <v>217</v>
+      </c>
+      <c r="H47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="11" customFormat="1" ht="18">
+      <c r="A48"/>
+      <c r="B48" t="s">
+        <v>218</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
         <v>89.99</v>
       </c>
-      <c r="G47" t="s">
+      <c r="F48" s="3">
+        <f>D48*E48</f>
+        <v>89.99</v>
+      </c>
+      <c r="G48" t="s">
         <v>220</v>
       </c>
-      <c r="H47"/>
-      <c r="I47"/>
-      <c r="J47" s="4">
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48" s="4">
         <v>41744</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="49" spans="1:10">
+      <c r="B49" t="s">
         <v>100</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>99</v>
       </c>
-      <c r="D48">
+      <c r="D49">
         <v>5</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E49" s="3">
         <v>29.99</v>
       </c>
-      <c r="F48" s="3">
-        <f t="shared" ref="F48:F61" si="3">D48*E48</f>
+      <c r="F49" s="3">
+        <f t="shared" ref="F49:F62" si="3">D49*E49</f>
         <v>149.94999999999999</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G49" t="s">
         <v>98</v>
       </c>
-      <c r="J48" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="10" t="s">
+      <c r="J49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="B50" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>104</v>
       </c>
-      <c r="D49">
+      <c r="D50">
         <v>2</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E50" s="3">
         <v>15</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F50" s="3">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G50" t="s">
         <v>101</v>
       </c>
-      <c r="J49" s="4">
-        <v>41690</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="J50" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="B51" t="s">
         <v>67</v>
       </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3">
+      <c r="E51" s="3"/>
+      <c r="F51" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
-      <c r="B51" s="11" t="s">
+    <row r="52" spans="1:10">
+      <c r="A52" s="11"/>
+      <c r="B52" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C52" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D51" s="11">
+      <c r="D52" s="11">
         <v>2</v>
       </c>
-      <c r="E51" s="12">
+      <c r="E52" s="12">
         <v>34.950000000000003</v>
       </c>
-      <c r="F51" s="12">
-        <f>D51*E51</f>
+      <c r="F52" s="12">
+        <f>D52*E52</f>
         <v>69.900000000000006</v>
       </c>
-      <c r="G51" s="11" t="s">
+      <c r="G52" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="H51" s="11" t="s">
+      <c r="H52" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I51" s="11" t="s">
+      <c r="I52" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="J51" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+      <c r="J52" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="B53" t="s">
         <v>77</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>79</v>
       </c>
-      <c r="D52">
+      <c r="D53">
         <v>2</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E53" s="3">
         <v>9.9499999999999993</v>
       </c>
-      <c r="F52" s="3">
-        <f>D52*E52</f>
+      <c r="F53" s="3">
+        <f>D53*E53</f>
         <v>19.899999999999999</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G53" t="s">
         <v>78</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H53" t="s">
         <v>80</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I53" t="s">
         <v>81</v>
       </c>
-      <c r="J52" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="J53" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="B54" t="s">
         <v>91</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>10</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E54" s="3">
         <v>1.46</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F54" s="3">
         <f t="shared" si="3"/>
         <v>14.6</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>93</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H54" t="s">
         <v>94</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I54" t="s">
         <v>95</v>
       </c>
-      <c r="J53" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="15" t="s">
+      <c r="J54" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="B55" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>114</v>
       </c>
-      <c r="D54">
+      <c r="D55">
         <v>2</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E55" s="3">
         <v>14.99</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F55" s="3">
         <f t="shared" si="3"/>
         <v>29.98</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G55" t="s">
         <v>113</v>
       </c>
-      <c r="J54" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="15" t="s">
+      <c r="J55" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="B56" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>116</v>
       </c>
-      <c r="D55">
+      <c r="D56">
         <v>4</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E56" s="3">
         <v>2.0299999999999998</v>
       </c>
-      <c r="F55" s="3">
-        <f>E55*D55</f>
+      <c r="F56" s="3">
+        <f>E56*D56</f>
         <v>8.1199999999999992</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G56" t="s">
         <v>115</v>
       </c>
-      <c r="J55" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+      <c r="J56" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="B57" t="s">
         <v>117</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>118</v>
       </c>
-      <c r="D56">
+      <c r="D57">
         <v>10</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E57" s="3">
         <v>1.018</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F57" s="3">
         <f t="shared" si="3"/>
         <v>10.18</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G57" t="s">
         <v>119</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I57" t="s">
         <v>127</v>
       </c>
-      <c r="J56" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+      <c r="J57" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="B58" t="s">
         <v>140</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>142</v>
       </c>
-      <c r="D57">
+      <c r="D58">
         <v>2</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E58" s="3">
         <v>24.99</v>
       </c>
-      <c r="F57" s="3">
+      <c r="F58" s="3">
         <f t="shared" si="3"/>
         <v>49.98</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G58" t="s">
         <v>141</v>
       </c>
-      <c r="J57" s="4">
-        <v>41711</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="J58" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="B59" t="s">
         <v>152</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>154</v>
-      </c>
-      <c r="D58">
-        <v>10</v>
-      </c>
-      <c r="E58" s="3">
-        <v>1</v>
-      </c>
-      <c r="F58" s="3">
-        <f>E58*D58</f>
-        <v>10</v>
-      </c>
-      <c r="G58" t="s">
-        <v>153</v>
-      </c>
-      <c r="J58" s="4">
-        <v>41711</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>151</v>
-      </c>
-      <c r="C59" t="s">
-        <v>150</v>
       </c>
       <c r="D59">
         <v>10</v>
@@ -2528,171 +2542,194 @@
         <v>10</v>
       </c>
       <c r="G59" t="s">
+        <v>153</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="B60" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" t="s">
+        <v>150</v>
+      </c>
+      <c r="D60">
+        <v>10</v>
+      </c>
+      <c r="E60" s="3">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3">
+        <f>E60*D60</f>
+        <v>10</v>
+      </c>
+      <c r="G60" t="s">
         <v>149</v>
       </c>
-      <c r="J59" s="4">
-        <v>41711</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+      <c r="J60" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15">
+      <c r="B61" t="s">
         <v>148</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C61" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60" s="3">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" s="3">
         <v>5.07</v>
       </c>
-      <c r="F60" s="3">
+      <c r="F61" s="3">
         <f t="shared" si="3"/>
         <v>5.07</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G61" t="s">
         <v>146</v>
       </c>
-      <c r="J60" s="17">
-        <v>41710</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+      <c r="J61" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="B62" t="s">
         <v>145</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>144</v>
       </c>
-      <c r="D61">
+      <c r="D62">
         <v>4</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E62" s="3">
         <v>1.36</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F62" s="3">
         <f t="shared" si="3"/>
         <v>5.44</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G62" t="s">
         <v>143</v>
       </c>
-      <c r="J61" s="17">
-        <v>41710</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+      <c r="J62" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="B63" t="s">
         <v>224</v>
       </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="B64" t="s">
         <v>225</v>
       </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
         <v>21</v>
       </c>
-      <c r="F64" s="3">
-        <f>SUM(F5:F61)</f>
-        <v>3932.86</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="F65" s="3">
+        <f>SUM(F5:F62)</f>
+        <v>3938.86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
         <v>26</v>
       </c>
-      <c r="F66" s="3">
-        <f>SUM(F37)</f>
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="F67" s="3">
+        <f>SUM(F38,F48,F42,F43,F26,F36)</f>
+        <v>1409.8200000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
         <v>25</v>
       </c>
-      <c r="F68" s="3">
-        <f>F64-F66</f>
-        <v>2767.86</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>68</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D73">
-        <v>1</v>
-      </c>
-      <c r="E73" s="3">
-        <v>23.75</v>
-      </c>
-      <c r="F73" s="3">
-        <f>D73*E73</f>
-        <v>23.75</v>
-      </c>
-      <c r="G73" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H73" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F69" s="3">
+        <f>F65-F67</f>
+        <v>2529.04</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
       <c r="B74" t="s">
         <v>68</v>
       </c>
-      <c r="C74" s="8" t="s">
-        <v>85</v>
+      <c r="C74" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
       <c r="E74" s="3">
-        <v>13.78</v>
+        <v>23.75</v>
       </c>
       <c r="F74" s="3">
         <f>D74*E74</f>
+        <v>23.75</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H74" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="B75" t="s">
+        <v>68</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75" s="3">
         <v>13.78</v>
       </c>
-      <c r="G74" s="7" t="s">
+      <c r="F75" s="3">
+        <f>D75*E75</f>
+        <v>13.78</v>
+      </c>
+      <c r="G75" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H75" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G29" r:id="rId1"/>
-    <hyperlink ref="G73" r:id="rId2" location="dl"/>
-    <hyperlink ref="G74" r:id="rId3"/>
+    <hyperlink ref="G30" r:id="rId1"/>
+    <hyperlink ref="G74" r:id="rId2" location="dl"/>
+    <hyperlink ref="G75" r:id="rId3"/>
     <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="C54" r:id="rId5" display="5V 3A BEC Step-Down Voltage Regulator"/>
-    <hyperlink ref="G30" r:id="rId6"/>
-    <hyperlink ref="G31" r:id="rId7"/>
-    <hyperlink ref="G33" r:id="rId8"/>
+    <hyperlink ref="C55" r:id="rId5" display="5V 3A BEC Step-Down Voltage Regulator"/>
+    <hyperlink ref="G31" r:id="rId6"/>
+    <hyperlink ref="G32" r:id="rId7"/>
+    <hyperlink ref="G34" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId9"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2705,20 +2742,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="56">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2750,11 +2787,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2771,7 +2808,8 @@
         <v>135</v>
       </c>
       <c r="F3" s="3">
-        <v>270</v>
+        <f>D3*E3</f>
+        <v>135</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>35</v>
@@ -2783,7 +2821,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="B4" t="s">
         <v>37</v>
       </c>
@@ -2791,13 +2829,14 @@
         <v>38</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
         <v>29.99</v>
       </c>
       <c r="F4" s="3">
-        <v>59.98</v>
+        <f>D4*E4</f>
+        <v>29.99</v>
       </c>
       <c r="G4" t="s">
         <v>39</v>
@@ -2806,7 +2845,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -2817,10 +2856,11 @@
         <v>0</v>
       </c>
       <c r="F5" s="3">
+        <f>D5*E5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2837,7 +2877,8 @@
         <v>7.81</v>
       </c>
       <c r="F7" s="3">
-        <v>15.62</v>
+        <f t="shared" ref="F7:F21" si="0">D7*E7</f>
+        <v>7.81</v>
       </c>
       <c r="G7" t="s">
         <v>46</v>
@@ -2846,7 +2887,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="B8" t="s">
         <v>44</v>
       </c>
@@ -2860,7 +2901,8 @@
         <v>7.81</v>
       </c>
       <c r="F8" s="3">
-        <v>15.62</v>
+        <f t="shared" si="0"/>
+        <v>7.81</v>
       </c>
       <c r="G8" t="s">
         <v>48</v>
@@ -2869,7 +2911,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" t="s">
         <v>49</v>
       </c>
@@ -2883,6 +2925,7 @@
         <v>7.81</v>
       </c>
       <c r="F9" s="3">
+        <f t="shared" si="0"/>
         <v>31.24</v>
       </c>
       <c r="G9" t="s">
@@ -2892,7 +2935,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="B10" t="s">
         <v>52</v>
       </c>
@@ -2906,7 +2949,8 @@
         <v>10.1</v>
       </c>
       <c r="F10" s="3">
-        <v>80.8</v>
+        <f t="shared" si="0"/>
+        <v>40.4</v>
       </c>
       <c r="G10" t="s">
         <v>53</v>
@@ -2915,7 +2959,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="B11" t="s">
         <v>54</v>
       </c>
@@ -2929,7 +2973,8 @@
         <v>1.68</v>
       </c>
       <c r="F11" s="3">
-        <v>13.44</v>
+        <f t="shared" si="0"/>
+        <v>6.72</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>56</v>
@@ -2938,7 +2983,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="B12" t="s">
         <v>57</v>
       </c>
@@ -2952,7 +2997,8 @@
         <v>2.9</v>
       </c>
       <c r="F12" s="3">
-        <v>23.2</v>
+        <f t="shared" si="0"/>
+        <v>11.6</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>58</v>
@@ -2961,7 +3007,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="B13" t="s">
         <v>59</v>
       </c>
@@ -2975,6 +3021,7 @@
         <v>1.44</v>
       </c>
       <c r="F13" s="3">
+        <f t="shared" si="0"/>
         <v>11.52</v>
       </c>
       <c r="G13" s="7" t="s">
@@ -2984,7 +3031,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="B14" t="s">
         <v>62</v>
       </c>
@@ -2998,7 +3045,8 @@
         <v>18.48</v>
       </c>
       <c r="F14" s="3">
-        <v>184.8</v>
+        <f t="shared" si="0"/>
+        <v>73.92</v>
       </c>
       <c r="G14" t="s">
         <v>97</v>
@@ -3007,7 +3055,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="B15" t="s">
         <v>64</v>
       </c>
@@ -3021,7 +3069,8 @@
         <v>3.16</v>
       </c>
       <c r="F15" s="3">
-        <v>15.8</v>
+        <f t="shared" si="0"/>
+        <v>6.32</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>128</v>
@@ -3030,7 +3079,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="B16" t="s">
         <v>96</v>
       </c>
@@ -3041,7 +3090,8 @@
         <v>4.74</v>
       </c>
       <c r="F16" s="3">
-        <v>28.44</v>
+        <f t="shared" si="0"/>
+        <v>9.48</v>
       </c>
       <c r="G16" t="s">
         <v>129</v>
@@ -3050,7 +3100,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="B17" t="s">
         <v>155</v>
       </c>
@@ -3064,7 +3114,8 @@
         <v>1.42</v>
       </c>
       <c r="F17" s="3">
-        <v>14.2</v>
+        <f t="shared" si="0"/>
+        <v>5.68</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>156</v>
@@ -3073,7 +3124,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="B18" t="s">
         <v>165</v>
       </c>
@@ -3087,7 +3138,8 @@
         <v>9.49</v>
       </c>
       <c r="F18" s="3">
-        <v>18.98</v>
+        <f t="shared" si="0"/>
+        <v>9.49</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>159</v>
@@ -3096,7 +3148,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="B19" s="18" t="s">
         <v>160</v>
       </c>
@@ -3110,11 +3162,11 @@
         <v>11.26</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" ref="F19:F21" si="0">D19*E19</f>
+        <f t="shared" si="0"/>
         <v>11.26</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="B20" t="s">
         <v>161</v>
       </c>
@@ -3132,7 +3184,7 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="B21" t="s">
         <v>166</v>
       </c>
@@ -3156,7 +3208,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="B22" t="s">
         <v>169</v>
       </c>
@@ -3170,7 +3222,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="B23" t="s">
         <v>171</v>
       </c>
@@ -3184,7 +3236,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="B24" t="s">
         <v>172</v>
       </c>
@@ -3195,7 +3247,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="B25" t="s">
         <v>174</v>
       </c>
@@ -3209,7 +3261,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="B26" t="s">
         <v>175</v>
       </c>
@@ -3223,7 +3275,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="B27" t="s">
         <v>176</v>
       </c>
@@ -3237,7 +3289,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="B28" t="s">
         <v>177</v>
       </c>
@@ -3251,7 +3303,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>179</v>
       </c>
@@ -3268,7 +3320,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="B30" t="s">
         <v>180</v>
       </c>
@@ -3289,7 +3341,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="B31" t="s">
         <v>182</v>
       </c>
@@ -3313,7 +3365,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="B32" t="s">
         <v>186</v>
       </c>
@@ -3337,7 +3389,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="B33" t="s">
         <v>189</v>
       </c>
@@ -3361,7 +3413,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="B34" t="s">
         <v>192</v>
       </c>
@@ -3385,7 +3437,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="B35" t="s">
         <v>195</v>
       </c>
@@ -3409,7 +3461,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="B36" t="s">
         <v>198</v>
       </c>
@@ -3433,7 +3485,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="B37" t="s">
         <v>201</v>
       </c>
@@ -3457,7 +3509,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -3478,7 +3530,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="5"/>
       <c r="B40" s="5" t="s">
         <v>28</v>
@@ -3509,7 +3561,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="5"/>
       <c r="B41" s="5" t="s">
         <v>31</v>
@@ -3540,7 +3592,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="B42" t="s">
         <v>105</v>
       </c>
@@ -3570,7 +3622,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="B43" t="s">
         <v>109</v>
       </c>
@@ -3600,7 +3652,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="B44" t="s">
         <v>125</v>
       </c>
@@ -3624,7 +3676,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="B45" t="s">
         <v>204</v>
       </c>
@@ -3648,7 +3700,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="B46" t="s">
         <v>137</v>
       </c>
@@ -3678,7 +3730,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="15">
       <c r="B47" s="20" t="s">
         <v>207</v>
       </c>
@@ -3699,12 +3751,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="J48" s="14"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -3721,7 +3773,7 @@
         <v>1165</v>
       </c>
       <c r="F49" s="3">
-        <f>D49*E49</f>
+        <f t="shared" ref="F49:F54" si="3">D49*E49</f>
         <v>1165</v>
       </c>
       <c r="G49" t="s">
@@ -3731,7 +3783,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="B50" t="s">
         <v>41</v>
       </c>
@@ -3743,18 +3795,20 @@
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="B51" t="s">
         <v>42</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J51" s="14" t="s">
@@ -3764,7 +3818,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="B52" t="s">
         <v>70</v>
       </c>
@@ -3778,7 +3832,7 @@
         <v>39</v>
       </c>
       <c r="F52" s="3">
-        <f>D52*E52</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="G52" t="s">
@@ -3788,7 +3842,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="18">
       <c r="B53" t="s">
         <v>209</v>
       </c>
@@ -3802,7 +3856,7 @@
         <v>79.790000000000006</v>
       </c>
       <c r="F53" s="3">
-        <f>D53*E53</f>
+        <f t="shared" si="3"/>
         <v>79.790000000000006</v>
       </c>
       <c r="G53" t="s">
@@ -3812,7 +3866,7 @@
         <v>41744</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="18">
       <c r="B54" t="s">
         <v>212</v>
       </c>
@@ -3826,7 +3880,7 @@
         <v>6.13</v>
       </c>
       <c r="F54" s="3">
-        <f>D54*E54</f>
+        <f t="shared" si="3"/>
         <v>6.13</v>
       </c>
       <c r="G54" t="s">
@@ -3836,19 +3890,19 @@
         <v>41744</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="18">
       <c r="C55" s="21"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="18">
       <c r="C56" s="21"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -3862,7 +3916,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="3">
-        <f>D57*E57</f>
+        <f t="shared" ref="F57:F71" si="4">D57*E57</f>
         <v>0</v>
       </c>
       <c r="G57" t="s">
@@ -3872,7 +3926,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11">
       <c r="B58" t="s">
         <v>215</v>
       </c>
@@ -3886,7 +3940,7 @@
         <v>169.99</v>
       </c>
       <c r="F58" s="3">
-        <f>D58*E58</f>
+        <f t="shared" si="4"/>
         <v>339.98</v>
       </c>
       <c r="G58" t="s">
@@ -3899,7 +3953,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="18">
       <c r="B59" t="s">
         <v>218</v>
       </c>
@@ -3913,7 +3967,7 @@
         <v>89.99</v>
       </c>
       <c r="F59" s="3">
-        <f>D59*E59</f>
+        <f t="shared" si="4"/>
         <v>89.99</v>
       </c>
       <c r="G59" t="s">
@@ -3923,7 +3977,7 @@
         <v>41744</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11">
       <c r="B60" t="s">
         <v>100</v>
       </c>
@@ -3937,7 +3991,7 @@
         <v>29.99</v>
       </c>
       <c r="F60" s="3">
-        <f>D60*E60</f>
+        <f t="shared" si="4"/>
         <v>119.96</v>
       </c>
       <c r="G60" s="7" t="s">
@@ -3947,7 +4001,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11">
       <c r="B61" s="15" t="s">
         <v>66</v>
       </c>
@@ -3961,7 +4015,7 @@
         <v>15</v>
       </c>
       <c r="F61" s="3">
-        <f>D61*E61</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="G61" t="s">
@@ -3971,17 +4025,17 @@
         <v>221</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11">
       <c r="B62" t="s">
         <v>67</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3">
-        <f t="shared" ref="F62:F71" si="3">D62*E62</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11">
       <c r="A63" s="22"/>
       <c r="B63" s="22" t="s">
         <v>73</v>
@@ -3996,7 +4050,7 @@
         <v>34.950000000000003</v>
       </c>
       <c r="F63" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>69.900000000000006</v>
       </c>
       <c r="G63" s="22" t="s">
@@ -4012,7 +4066,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11">
       <c r="B64" t="s">
         <v>77</v>
       </c>
@@ -4026,7 +4080,7 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19.899999999999999</v>
       </c>
       <c r="G64" t="s">
@@ -4042,7 +4096,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="B65" t="s">
         <v>91</v>
       </c>
@@ -4056,7 +4110,7 @@
         <v>1.46</v>
       </c>
       <c r="F65" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14.6</v>
       </c>
       <c r="G65" t="s">
@@ -4072,7 +4126,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="B66" s="15" t="s">
         <v>102</v>
       </c>
@@ -4086,7 +4140,7 @@
         <v>14.99</v>
       </c>
       <c r="F66" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29.98</v>
       </c>
       <c r="G66" t="s">
@@ -4096,7 +4150,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="B67" s="15" t="s">
         <v>103</v>
       </c>
@@ -4110,7 +4164,7 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="F67" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.1199999999999992</v>
       </c>
       <c r="G67" t="s">
@@ -4120,7 +4174,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="B68" t="s">
         <v>140</v>
       </c>
@@ -4134,7 +4188,7 @@
         <v>24.99</v>
       </c>
       <c r="F68" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>49.98</v>
       </c>
       <c r="G68" t="s">
@@ -4144,7 +4198,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="B69" t="s">
         <v>152</v>
       </c>
@@ -4158,7 +4212,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G69" t="s">
@@ -4168,7 +4222,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="B70" t="s">
         <v>151</v>
       </c>
@@ -4182,7 +4236,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G70" t="s">
@@ -4192,7 +4246,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="B71" t="s">
         <v>145</v>
       </c>
@@ -4206,7 +4260,7 @@
         <v>1.36</v>
       </c>
       <c r="F71" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.44</v>
       </c>
       <c r="G71" t="s">
@@ -4216,7 +4270,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="22"/>
       <c r="B72" s="22" t="s">
         <v>222</v>
@@ -4234,7 +4288,7 @@
       <c r="I72" s="22"/>
       <c r="J72" s="22"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="B73" t="s">
         <v>224</v>
       </c>
@@ -4242,7 +4296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="B74" t="s">
         <v>225</v>
       </c>
@@ -4250,7 +4304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>26</v>
       </c>
@@ -4259,16 +4313,16 @@
         <v>1403.8200000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>25</v>
       </c>
       <c r="F78" s="3">
         <f>SUM(F3:F71) - F76</f>
-        <v>2110.6851999999999</v>
+        <v>1714.0252</v>
       </c>
     </row>
   </sheetData>
@@ -4291,6 +4345,7 @@
     <hyperlink ref="C34" r:id="rId16" tooltip="Add item to current order" display="http://www.mcmaster.com/nav/enter.asp?partnum=94510A040"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>